<commit_message>
Not sure why but I'm doing vectors now
</commit_message>
<xml_diff>
--- a/docs/Hardware.xlsx
+++ b/docs/Hardware.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\Aznable\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3FBFE3B-C280-4EE8-81E3-50FAD27BE6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F768E68-CB2A-4795-853D-F2E6F25048D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{8387191E-7D8B-4623-897E-A5E3E75A545C}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Casval" sheetId="2" r:id="rId2"/>
     <sheet name="Sound" sheetId="3" r:id="rId3"/>
     <sheet name="Tilemap" sheetId="4" r:id="rId4"/>
+    <sheet name="Vector" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="SCREEN_BORDER_WIDTH">Hardware!$M$3</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="240">
   <si>
     <t>HEIGHT</t>
   </si>
@@ -58,9 +59,6 @@
   </si>
   <si>
     <t>0x0000</t>
-  </si>
-  <si>
-    <t>0x4000</t>
   </si>
   <si>
     <t>Program ROM</t>
@@ -775,6 +773,54 @@
   </si>
   <si>
     <t>Char Palette RAM B</t>
+  </si>
+  <si>
+    <t>Vector instruction RAM area</t>
+  </si>
+  <si>
+    <t>=- Stores lists of line drawing instructions</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>Intensity / Colour?</t>
+  </si>
+  <si>
+    <t>4 bits for intensity , 4 for colour palette index?</t>
+  </si>
+  <si>
+    <t>Byte</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Number of points making up this polyline</t>
+  </si>
+  <si>
+    <t>Start X</t>
+  </si>
+  <si>
+    <t>Start Y</t>
+  </si>
+  <si>
+    <t>Move to X</t>
+  </si>
+  <si>
+    <t>Move to Y</t>
+  </si>
+  <si>
+    <t>Vulcan (Vector engine)</t>
+  </si>
+  <si>
+    <t>Line RAM</t>
+  </si>
+  <si>
+    <t>0x2000</t>
   </si>
 </sst>
 </file>
@@ -1146,9 +1192,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1186,7 +1232,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1292,7 +1338,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1434,7 +1480,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1444,8 +1490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C319FCBA-55CF-4FE5-A99F-6174DD3BEDA9}">
   <dimension ref="B1:P96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+    <sheetView tabSelected="1" topLeftCell="B27" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1469,53 +1515,53 @@
   <sheetData>
     <row r="1" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B1" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B2" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="F2" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="19" t="s">
-        <v>34</v>
-      </c>
       <c r="G2" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>31</v>
-      </c>
       <c r="J2" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L2" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="23" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F3" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I3))</f>
@@ -1534,7 +1580,7 @@
         <v>32768</v>
       </c>
       <c r="J3" s="23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L3" s="18" t="s">
         <v>2</v>
@@ -1549,17 +1595,17 @@
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B4" s="24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" s="23" t="str">
-        <f t="shared" ref="D4:D51" si="2">F3</f>
+        <f t="shared" ref="D4:D46" si="2">F3</f>
         <v>0x8000</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I4))</f>
@@ -1578,7 +1624,7 @@
         <v>32769</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L4" s="18" t="s">
         <v>1</v>
@@ -1603,7 +1649,7 @@
         <v>0x8001</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I5))</f>
@@ -1622,7 +1668,7 @@
         <v>32770</v>
       </c>
       <c r="J5" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L5" s="18" t="s">
         <v>0</v>
@@ -1643,7 +1689,7 @@
         <v>0x8002</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F6" s="27" t="str">
         <f t="shared" ref="F6" si="6">_xlfn.CONCAT("0x",DEC2HEX(I6))</f>
@@ -1662,7 +1708,7 @@
         <v>32896</v>
       </c>
       <c r="J6" s="27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.2">
@@ -1673,7 +1719,7 @@
         <v>0x8080</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F7" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I7))</f>
@@ -1692,10 +1738,10 @@
         <v>32928</v>
       </c>
       <c r="J7" s="23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L7" s="20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O7" s="18">
         <f>O4*O5</f>
@@ -1710,7 +1756,7 @@
         <v>0x80A0</v>
       </c>
       <c r="E8" s="27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F8" s="27" t="str">
         <f t="shared" ref="F8" si="8">_xlfn.CONCAT("0x",DEC2HEX(I8))</f>
@@ -1729,10 +1775,10 @@
         <v>32960</v>
       </c>
       <c r="J8" s="27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L8" s="28" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="M8" s="28">
         <v>256</v>
@@ -1746,7 +1792,7 @@
         <v>0x80C0</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F9" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I9))</f>
@@ -1765,10 +1811,10 @@
         <v>32976</v>
       </c>
       <c r="J9" s="23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L9" s="18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M9" s="18">
         <v>8</v>
@@ -1782,7 +1828,7 @@
         <v>0x80D0</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F10" s="27" t="str">
         <f t="shared" ref="F10" si="12">_xlfn.CONCAT("0x",DEC2HEX(I10))</f>
@@ -1801,10 +1847,10 @@
         <v>33024</v>
       </c>
       <c r="J10" s="27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L10" s="18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M10" s="18">
         <v>8</v>
@@ -1818,7 +1864,7 @@
         <v>0x8100</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I11))</f>
@@ -1837,10 +1883,10 @@
         <v>33216</v>
       </c>
       <c r="J11" s="23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L11" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M11" s="18">
         <v>1</v>
@@ -1854,7 +1900,7 @@
         <v>0x81C0</v>
       </c>
       <c r="E12" s="27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F12" s="27" t="str">
         <f t="shared" ref="F12" si="14">_xlfn.CONCAT("0x",DEC2HEX(I12))</f>
@@ -1873,10 +1919,10 @@
         <v>33280</v>
       </c>
       <c r="J12" s="27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L12" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M12" s="29">
         <f>M9*M10*M11</f>
@@ -1891,7 +1937,7 @@
         <v>0x8200</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I13))</f>
@@ -1910,10 +1956,10 @@
         <v>33376</v>
       </c>
       <c r="J13" s="23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L13" s="18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M13" s="18">
         <f>M12/8</f>
@@ -1928,7 +1974,7 @@
         <v>0x8260</v>
       </c>
       <c r="E14" s="27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F14" s="27" t="str">
         <f t="shared" ref="F14" si="19">_xlfn.CONCAT("0x",DEC2HEX(I14))</f>
@@ -1947,10 +1993,10 @@
         <v>33408</v>
       </c>
       <c r="J14" s="27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L14" s="29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="M14" s="29">
         <f>M8*M13</f>
@@ -1965,7 +2011,7 @@
         <v>0x8280</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F15" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I15))</f>
@@ -1984,7 +2030,7 @@
         <v>33504</v>
       </c>
       <c r="J15" s="23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.2">
@@ -1995,7 +2041,7 @@
         <v>0x82E0</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F16" s="27" t="str">
         <f t="shared" ref="F16" si="20">_xlfn.CONCAT("0x",DEC2HEX(I16))</f>
@@ -2014,10 +2060,10 @@
         <v>33536</v>
       </c>
       <c r="J16" s="27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L16" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.2">
@@ -2028,7 +2074,7 @@
         <v>0x8300</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F17" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I17))</f>
@@ -2047,10 +2093,10 @@
         <v>33584</v>
       </c>
       <c r="J17" s="23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L17" s="28" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="M17" s="28">
         <v>256</v>
@@ -2068,7 +2114,7 @@
         <v>0x8330</v>
       </c>
       <c r="E18" s="27" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F18" s="27" t="str">
         <f t="shared" ref="F18" si="25">_xlfn.CONCAT("0x",DEC2HEX(I18))</f>
@@ -2087,10 +2133,10 @@
         <v>33664</v>
       </c>
       <c r="J18" s="27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L18" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M18" s="18">
         <v>32</v>
@@ -2104,7 +2150,7 @@
         <v>0x8380</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F19" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I19))</f>
@@ -2123,10 +2169,10 @@
         <v>33760</v>
       </c>
       <c r="J19" s="23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L19" s="29" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M19" s="29">
         <f>M18</f>
@@ -2141,7 +2187,7 @@
         <v>0x83E0</v>
       </c>
       <c r="E20" s="27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F20" s="27" t="str">
         <f t="shared" ref="F20" si="26">_xlfn.CONCAT("0x",DEC2HEX(I20))</f>
@@ -2160,10 +2206,10 @@
         <v>33792</v>
       </c>
       <c r="J20" s="27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L20" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="M20" s="18">
         <f>M19/8</f>
@@ -2178,7 +2224,7 @@
         <v>0x8400</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F21" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I21))</f>
@@ -2197,10 +2243,10 @@
         <v>33804</v>
       </c>
       <c r="J21" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L21" s="29" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M21" s="29">
         <f>M17*M20</f>
@@ -2215,7 +2261,7 @@
         <v>0x840C</v>
       </c>
       <c r="E22" s="27" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F22" s="27" t="str">
         <f t="shared" ref="F22" si="32">_xlfn.CONCAT("0x",DEC2HEX(I22))</f>
@@ -2234,7 +2280,7 @@
         <v>33920</v>
       </c>
       <c r="J22" s="27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.2">
@@ -2245,7 +2291,7 @@
         <v>0x8480</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F23" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I23))</f>
@@ -2264,10 +2310,10 @@
         <v>33968</v>
       </c>
       <c r="J23" s="23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L23" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.2">
@@ -2278,7 +2324,7 @@
         <v>0x84B0</v>
       </c>
       <c r="E24" s="27" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F24" s="27" t="str">
         <f t="shared" ref="F24" si="33">_xlfn.CONCAT("0x",DEC2HEX(I24))</f>
@@ -2297,10 +2343,10 @@
         <v>34048</v>
       </c>
       <c r="J24" s="27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L24" s="28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M24" s="28">
         <v>4</v>
@@ -2314,7 +2360,7 @@
         <v>0x8500</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F25" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I25))</f>
@@ -2333,16 +2379,16 @@
         <v>34064</v>
       </c>
       <c r="J25" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L25" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M25" s="18">
         <v>16</v>
       </c>
       <c r="N25" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.2">
@@ -2353,7 +2399,7 @@
         <v>0x8510</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F26" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I26))</f>
@@ -2372,10 +2418,10 @@
         <v>34080</v>
       </c>
       <c r="J26" s="23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L26" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M26" s="18">
         <v>32</v>
@@ -2389,7 +2435,7 @@
         <v>0x8520</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F27" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I27))</f>
@@ -2408,10 +2454,10 @@
         <v>34096</v>
       </c>
       <c r="J27" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L27" s="29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M27" s="29">
         <f>M25*M26</f>
@@ -2426,7 +2472,7 @@
         <v>0x8530</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" s="23" t="str">
         <f t="shared" ref="F28" si="37">_xlfn.CONCAT("0x",DEC2HEX(I28))</f>
@@ -2445,10 +2491,10 @@
         <v>34097</v>
       </c>
       <c r="J28" s="23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L28" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M28" s="18">
         <f>M27/8</f>
@@ -2463,7 +2509,7 @@
         <v>0x8531</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29" s="23" t="str">
         <f t="shared" ref="F29" si="40">_xlfn.CONCAT("0x",DEC2HEX(I29))</f>
@@ -2482,10 +2528,10 @@
         <v>34098</v>
       </c>
       <c r="J29" s="23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L29" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M29" s="29">
         <f>M28*M24</f>
@@ -2500,7 +2546,7 @@
         <v>0x8532</v>
       </c>
       <c r="E30" s="27" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F30" s="27" t="str">
         <f t="shared" ref="F30" si="43">_xlfn.CONCAT("0x",DEC2HEX(I30))</f>
@@ -2519,20 +2565,20 @@
         <v>34176</v>
       </c>
       <c r="J30" s="27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B31" s="24"/>
       <c r="C31" s="47" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D31" s="23" t="str">
         <f>F30</f>
         <v>0x8580</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F31" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I31))</f>
@@ -2551,13 +2597,13 @@
         <v>34192</v>
       </c>
       <c r="J31" s="23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L31" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N31" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.2">
@@ -2568,7 +2614,7 @@
         <v>0x8590</v>
       </c>
       <c r="E32" s="23" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F32" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I32))</f>
@@ -2587,10 +2633,10 @@
         <v>34196</v>
       </c>
       <c r="J32" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L32" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M32" s="28">
         <v>64</v>
@@ -2604,7 +2650,7 @@
         <v>0x8594</v>
       </c>
       <c r="E33" s="27" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F33" s="27" t="str">
         <f t="shared" ref="F33" si="49">_xlfn.CONCAT("0x",DEC2HEX(I33))</f>
@@ -2623,10 +2669,10 @@
         <v>34304</v>
       </c>
       <c r="J33" s="27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L33" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M33" s="18">
         <v>16</v>
@@ -2635,7 +2681,7 @@
     <row r="34" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B34" s="24"/>
       <c r="C34" s="44" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D34" s="23" t="str">
         <f>F33</f>
@@ -2662,10 +2708,10 @@
         <v>34320</v>
       </c>
       <c r="J34" s="23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L34" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M34" s="18">
         <v>16</v>
@@ -2699,16 +2745,16 @@
         <v>35088</v>
       </c>
       <c r="J35" s="23" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L35" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M35" s="18">
         <v>8</v>
       </c>
       <c r="N35" s="18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.2">
@@ -2719,7 +2765,7 @@
         <v>0x8910</v>
       </c>
       <c r="E36" s="27" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F36" s="27" t="str">
         <f t="shared" ref="F36" si="54">_xlfn.CONCAT("0x",DEC2HEX(I36))</f>
@@ -2738,10 +2784,10 @@
         <v>35328</v>
       </c>
       <c r="J36" s="27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L36" s="29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M36" s="29">
         <f>M33*M34*M35</f>
@@ -2751,14 +2797,14 @@
     <row r="37" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B37" s="24"/>
       <c r="C37" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D37" s="23" t="str">
         <f>F36</f>
         <v>0x8A00</v>
       </c>
       <c r="E37" s="23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F37" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I37))</f>
@@ -2777,10 +2823,10 @@
         <v>37376</v>
       </c>
       <c r="J37" s="23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L37" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M37" s="18">
         <f>M36/8</f>
@@ -2795,7 +2841,7 @@
         <v>0x9200</v>
       </c>
       <c r="E38" s="23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F38" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I38))</f>
@@ -2814,10 +2860,10 @@
         <v>39424</v>
       </c>
       <c r="J38" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L38" s="29" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M38" s="29">
         <f>M32*M37</f>
@@ -2832,7 +2878,7 @@
         <v>0x9A00</v>
       </c>
       <c r="E39" s="23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F39" s="23" t="str">
         <f t="shared" ref="F39" si="57">_xlfn.CONCAT("0x",DEC2HEX(I39))</f>
@@ -2851,7 +2897,7 @@
         <v>41472</v>
       </c>
       <c r="J39" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.2">
@@ -2862,7 +2908,7 @@
         <v>0xA200</v>
       </c>
       <c r="E40" s="23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F40" s="23" t="str">
         <f t="shared" ref="F40:F44" si="61">_xlfn.CONCAT("0x",DEC2HEX(I40))</f>
@@ -2881,10 +2927,10 @@
         <v>43520</v>
       </c>
       <c r="J40" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L40" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.2">
@@ -2895,7 +2941,7 @@
         <v>0xAA00</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F41" s="23" t="str">
         <f t="shared" ref="F41" si="65">_xlfn.CONCAT("0x",DEC2HEX(I41))</f>
@@ -2914,10 +2960,10 @@
         <v>43776</v>
       </c>
       <c r="J41" s="23" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="L41" s="28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M41" s="28">
         <v>32</v>
@@ -2931,7 +2977,7 @@
         <v>0xAB00</v>
       </c>
       <c r="E42" s="23" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F42" s="23" t="str">
         <f t="shared" si="61"/>
@@ -2950,10 +2996,10 @@
         <v>44032</v>
       </c>
       <c r="J42" s="23" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L42" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M42" s="18">
         <v>1</v>
@@ -2967,7 +3013,7 @@
         <v>0xAC00</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F43" s="23" t="str">
         <f t="shared" ref="F43" si="69">_xlfn.CONCAT("0x",DEC2HEX(I43))</f>
@@ -2986,10 +3032,10 @@
         <v>44288</v>
       </c>
       <c r="J43" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L43" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M43" s="18">
         <v>1</v>
@@ -3003,7 +3049,7 @@
         <v>0xAD00</v>
       </c>
       <c r="E44" s="27" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F44" s="27" t="str">
         <f t="shared" si="61"/>
@@ -3022,10 +3068,10 @@
         <v>45056</v>
       </c>
       <c r="J44" s="27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L44" s="18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M44" s="18">
         <v>2</v>
@@ -3034,7 +3080,7 @@
     <row r="45" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B45" s="24"/>
       <c r="C45" s="33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D45" s="23" t="str">
         <f>F44</f>
@@ -3061,10 +3107,10 @@
         <v>45184</v>
       </c>
       <c r="J45" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L45" s="18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M45" s="18">
         <v>2</v>
@@ -3078,7 +3124,7 @@
         <v>0xB080</v>
       </c>
       <c r="E46" s="27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F46" s="27" t="str">
         <f t="shared" si="73"/>
@@ -3097,10 +3143,10 @@
         <v>46080</v>
       </c>
       <c r="J46" s="27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L46" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M46" s="18">
         <v>1</v>
@@ -3134,10 +3180,10 @@
         <v>46084</v>
       </c>
       <c r="J47" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L47" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M47" s="18">
         <v>9</v>
@@ -3151,7 +3197,7 @@
         <v>0xB404</v>
       </c>
       <c r="E48" s="27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F48" s="27" t="str">
         <f t="shared" si="78"/>
@@ -3170,10 +3216,10 @@
         <v>47104</v>
       </c>
       <c r="J48" s="27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L48" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M48" s="18">
         <v>7</v>
@@ -3195,7 +3241,7 @@
         <v>0xC000</v>
       </c>
       <c r="G49" s="23">
-        <f t="shared" ref="G49:H51" si="82">HEX2DEC(MID(D49, 3, LEN(D49)-2))</f>
+        <f t="shared" ref="G49:H50" si="82">HEX2DEC(MID(D49, 3, LEN(D49)-2))</f>
         <v>47104</v>
       </c>
       <c r="H49" s="23">
@@ -3207,30 +3253,30 @@
         <v>49152</v>
       </c>
       <c r="J49" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L49" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M49" s="18">
         <v>9</v>
       </c>
     </row>
     <row r="50" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B50" s="36"/>
+      <c r="B50" s="24"/>
       <c r="C50" s="37" t="s">
-        <v>41</v>
+        <v>237</v>
       </c>
       <c r="D50" s="23" t="str">
         <f>F49</f>
         <v>0xC000</v>
       </c>
       <c r="E50" s="23" t="s">
-        <v>6</v>
+        <v>239</v>
       </c>
       <c r="F50" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I50))</f>
-        <v>0x10000</v>
+        <v>0xE000</v>
       </c>
       <c r="G50" s="23">
         <f t="shared" si="82"/>
@@ -3238,14 +3284,14 @@
       </c>
       <c r="H50" s="23">
         <f t="shared" si="82"/>
-        <v>16384</v>
+        <v>8192</v>
       </c>
       <c r="I50" s="23">
         <f>G50+H50</f>
-        <v>65536</v>
+        <v>57344</v>
       </c>
       <c r="J50" s="23" t="s">
-        <v>17</v>
+        <v>238</v>
       </c>
       <c r="L50" s="29" t="s">
         <v>4</v>
@@ -3256,38 +3302,35 @@
       </c>
     </row>
     <row r="51" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B51" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="C51" s="40" t="s">
-        <v>47</v>
+      <c r="B51" s="36"/>
+      <c r="C51" s="37" t="s">
+        <v>40</v>
       </c>
       <c r="D51" s="23" t="str">
-        <f t="shared" si="2"/>
-        <v>0x10000</v>
-      </c>
-      <c r="E51" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M29))</f>
-        <v>0x100</v>
+        <f>F50</f>
+        <v>0xE000</v>
+      </c>
+      <c r="E51" s="23" t="s">
+        <v>239</v>
       </c>
       <c r="F51" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I51))</f>
-        <v>0x10100</v>
+        <v>0x10000</v>
       </c>
       <c r="G51" s="23">
-        <f t="shared" si="82"/>
-        <v>65536</v>
+        <f t="shared" ref="G51" si="83">HEX2DEC(MID(D51, 3, LEN(D51)-2))</f>
+        <v>57344</v>
       </c>
       <c r="H51" s="23">
-        <f t="shared" si="82"/>
-        <v>256</v>
+        <f t="shared" ref="H51" si="84">HEX2DEC(MID(E51, 3, LEN(E51)-2))</f>
+        <v>8192</v>
       </c>
       <c r="I51" s="23">
         <f>G51+H51</f>
-        <v>65792</v>
+        <v>65536</v>
       </c>
       <c r="J51" s="23" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="L51" s="18" t="s">
         <v>3</v>
@@ -3298,95 +3341,126 @@
       </c>
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B52" s="39" t="s">
-        <v>133</v>
-      </c>
       <c r="L52" s="29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M52" s="29">
         <f>M41*M51</f>
         <v>128</v>
       </c>
     </row>
-    <row r="53" spans="2:16" ht="15" x14ac:dyDescent="0.25">
-      <c r="B53" s="39"/>
-      <c r="C53"/>
-      <c r="D53"/>
-      <c r="E53"/>
-      <c r="F53"/>
-      <c r="G53"/>
-      <c r="H53"/>
-      <c r="I53"/>
-      <c r="J53"/>
+    <row r="53" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B53" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="C53" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="D53" s="23" t="str">
+        <f>F50</f>
+        <v>0xE000</v>
+      </c>
+      <c r="E53" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M29))</f>
+        <v>0x100</v>
+      </c>
+      <c r="F53" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I53))</f>
+        <v>0xE100</v>
+      </c>
+      <c r="G53" s="23">
+        <f>HEX2DEC(MID(D53, 3, LEN(D53)-2))</f>
+        <v>57344</v>
+      </c>
+      <c r="H53" s="23">
+        <f>HEX2DEC(MID(E53, 3, LEN(E53)-2))</f>
+        <v>256</v>
+      </c>
+      <c r="I53" s="23">
+        <f>G53+H53</f>
+        <v>57600</v>
+      </c>
+      <c r="J53" s="23" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="54" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B54" s="39"/>
-      <c r="C54" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="D54" s="23"/>
-      <c r="E54" s="23" t="str">
+      <c r="B54" s="39" t="s">
+        <v>132</v>
+      </c>
+      <c r="L54" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="M54" s="18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="55" spans="2:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="B55" s="39"/>
+      <c r="C55"/>
+      <c r="D55"/>
+      <c r="E55"/>
+      <c r="F55"/>
+      <c r="G55"/>
+      <c r="H55"/>
+      <c r="I55"/>
+      <c r="J55"/>
+      <c r="L55" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="M55" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B56" s="39"/>
+      <c r="C56" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="D56" s="23"/>
+      <c r="E56" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(M38))</f>
         <v>0x4000</v>
       </c>
-      <c r="F54" s="23"/>
-      <c r="G54" s="23"/>
-      <c r="H54" s="23">
-        <f>HEX2DEC(MID(E54, 3, LEN(E54)-2))</f>
+      <c r="F56" s="23"/>
+      <c r="G56" s="23"/>
+      <c r="H56" s="23">
+        <f>HEX2DEC(MID(E56, 3, LEN(E56)-2))</f>
         <v>16384</v>
       </c>
-      <c r="I54" s="23"/>
-      <c r="J54" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="L54" s="20" t="s">
+      <c r="I56" s="23"/>
+      <c r="J56" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="L56" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="M54" s="18" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="55" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B55" s="39"/>
-      <c r="C55" s="35"/>
-      <c r="D55" s="23"/>
-      <c r="E55" s="23" t="str">
+      <c r="M56" s="18">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="57" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B57" s="39"/>
+      <c r="C57" s="35"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(M71))</f>
         <v>0x800</v>
       </c>
-      <c r="F55" s="23"/>
-      <c r="G55" s="23"/>
-      <c r="H55" s="23">
-        <f>HEX2DEC(MID(E55, 3, LEN(E55)-2))</f>
+      <c r="F57" s="23"/>
+      <c r="G57" s="23"/>
+      <c r="H57" s="23">
+        <f>HEX2DEC(MID(E57, 3, LEN(E57)-2))</f>
         <v>2048</v>
       </c>
-      <c r="I55" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="J55" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="L55" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="M55" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B56" s="39"/>
-      <c r="L56" s="18" t="s">
+      <c r="I57" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="J57" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="L57" s="28" t="s">
         <v>66</v>
-      </c>
-      <c r="M56" s="18">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="57" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B57" s="39"/>
-      <c r="L57" s="28" t="s">
-        <v>67</v>
       </c>
       <c r="M57" s="28">
         <v>16</v>
@@ -3394,25 +3468,8 @@
     </row>
     <row r="58" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B58" s="39"/>
-      <c r="C58" s="40" t="s">
-        <v>145</v>
-      </c>
-      <c r="D58" s="23"/>
-      <c r="E58" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="F58" s="23"/>
-      <c r="G58" s="23"/>
-      <c r="H58" s="23">
-        <f t="shared" ref="H58" si="83">HEX2DEC(MID(E58, 3, LEN(E58)-2))</f>
-        <v>131072</v>
-      </c>
-      <c r="I58" s="23"/>
-      <c r="J58" s="23" t="s">
-        <v>145</v>
-      </c>
       <c r="L58" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M58" s="18">
         <f>M55*M56*M57</f>
@@ -3421,25 +3478,8 @@
     </row>
     <row r="59" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B59" s="39"/>
-      <c r="C59" s="40" t="s">
-        <v>158</v>
-      </c>
-      <c r="D59" s="23"/>
-      <c r="E59" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="F59" s="23"/>
-      <c r="G59" s="23"/>
-      <c r="H59" s="23">
-        <f t="shared" ref="H59" si="84">HEX2DEC(MID(E59, 3, LEN(E59)-2))</f>
-        <v>65536</v>
-      </c>
-      <c r="I59" s="23"/>
-      <c r="J59" s="23" t="s">
-        <v>158</v>
-      </c>
       <c r="L59" s="18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M59" s="18">
         <f>M58/8</f>
@@ -3448,23 +3488,57 @@
     </row>
     <row r="60" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B60" s="39"/>
+      <c r="C60" s="40" t="s">
+        <v>144</v>
+      </c>
+      <c r="D60" s="23"/>
+      <c r="E60" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="F60" s="23"/>
+      <c r="G60" s="23"/>
+      <c r="H60" s="23">
+        <f t="shared" ref="H60" si="85">HEX2DEC(MID(E60, 3, LEN(E60)-2))</f>
+        <v>131072</v>
+      </c>
+      <c r="I60" s="23"/>
+      <c r="J60" s="23" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="61" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B61" s="39"/>
+      <c r="C61" s="40" t="s">
+        <v>157</v>
+      </c>
+      <c r="D61" s="23"/>
+      <c r="E61" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="F61" s="23"/>
+      <c r="G61" s="23"/>
+      <c r="H61" s="23">
+        <f t="shared" ref="H61" si="86">HEX2DEC(MID(E61, 3, LEN(E61)-2))</f>
+        <v>65536</v>
+      </c>
+      <c r="I61" s="23"/>
+      <c r="J61" s="23" t="s">
+        <v>157</v>
+      </c>
       <c r="L61" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M61" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="P61" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="62" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B62" s="39"/>
       <c r="L62" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M62" s="18">
         <v>32</v>
@@ -3476,6 +3550,29 @@
     </row>
     <row r="63" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B63" s="39"/>
+      <c r="C63" s="37" t="s">
+        <v>237</v>
+      </c>
+      <c r="D63" s="23"/>
+      <c r="E63" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="F63" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I63))</f>
+        <v>0x10000</v>
+      </c>
+      <c r="G63" s="23"/>
+      <c r="H63" s="23">
+        <f t="shared" ref="H63" si="87">HEX2DEC(MID(E63, 3, LEN(E63)-2))</f>
+        <v>65536</v>
+      </c>
+      <c r="I63" s="23">
+        <f>G63+H63</f>
+        <v>65536</v>
+      </c>
+      <c r="J63" s="23" t="s">
+        <v>238</v>
+      </c>
       <c r="L63" s="28" t="s">
         <v>4</v>
       </c>
@@ -3486,7 +3583,7 @@
     <row r="64" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B64" s="39"/>
       <c r="L64" s="18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M64" s="18">
         <f>M62*M63</f>
@@ -3496,7 +3593,7 @@
     <row r="65" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B65" s="39"/>
       <c r="L65" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M65" s="18">
         <f>M64/8</f>
@@ -3509,40 +3606,40 @@
     <row r="67" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B67" s="39"/>
       <c r="L67" s="20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M67" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="68" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B68" s="39"/>
       <c r="L68" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M68" s="18">
         <v>512</v>
       </c>
       <c r="N68" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="69" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B69" s="39"/>
       <c r="L69" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M69" s="28">
         <v>32</v>
       </c>
       <c r="N69" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="70" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B70" s="39"/>
       <c r="L70" s="29" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M70" s="18">
         <f>M68*M69</f>
@@ -3552,7 +3649,7 @@
     <row r="71" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B71" s="39"/>
       <c r="L71" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M71" s="18">
         <f>M70/8</f>
@@ -3565,29 +3662,31 @@
     <row r="73" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B73" s="39"/>
       <c r="L73" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="74" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B74" s="41"/>
+      <c r="B74" s="39"/>
       <c r="L74" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M74" s="18">
         <v>8</v>
       </c>
     </row>
     <row r="75" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B75" s="39"/>
       <c r="L75" s="18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M75" s="18">
         <v>8</v>
       </c>
     </row>
     <row r="76" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B76" s="41"/>
       <c r="L76" s="18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M76" s="18">
         <v>8</v>
@@ -3595,7 +3694,7 @@
     </row>
     <row r="77" spans="2:14" x14ac:dyDescent="0.2">
       <c r="L77" s="18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M77" s="18">
         <v>8</v>
@@ -3603,7 +3702,7 @@
     </row>
     <row r="78" spans="2:14" x14ac:dyDescent="0.2">
       <c r="L78" s="43" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M78" s="43">
         <v>96</v>
@@ -3611,7 +3710,7 @@
     </row>
     <row r="79" spans="2:14" x14ac:dyDescent="0.2">
       <c r="L79" s="29" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="M79" s="29">
         <f>SUM(M74:M78)</f>
@@ -3620,7 +3719,7 @@
     </row>
     <row r="80" spans="2:14" x14ac:dyDescent="0.2">
       <c r="L80" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M80" s="18">
         <f>M79/8</f>
@@ -3629,34 +3728,34 @@
     </row>
     <row r="82" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L82" s="20" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="83" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L83" s="18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M83" s="18">
         <v>32</v>
       </c>
       <c r="N83" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="84" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L84" s="18" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="M84" s="18">
         <v>24</v>
       </c>
       <c r="N84" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="85" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L85" s="18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M85" s="18">
         <v>8</v>
@@ -3664,7 +3763,7 @@
     </row>
     <row r="86" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L86" s="29" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M86" s="29">
         <f>M83*M84*M85</f>
@@ -3673,7 +3772,7 @@
     </row>
     <row r="87" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L87" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M87" s="18">
         <f>M86/8</f>
@@ -3682,12 +3781,12 @@
     </row>
     <row r="89" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L89" s="20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="90" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L90" s="28" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M90" s="28">
         <v>64</v>
@@ -3695,7 +3794,7 @@
     </row>
     <row r="91" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L91" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M91" s="18">
         <v>16</v>
@@ -3703,7 +3802,7 @@
     </row>
     <row r="92" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L92" s="18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="M92" s="18">
         <v>16</v>
@@ -3711,18 +3810,18 @@
     </row>
     <row r="93" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L93" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="M93" s="18">
         <v>16</v>
       </c>
       <c r="N93" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="94" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L94" s="29" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="M94" s="29">
         <f>M91*M92*M93</f>
@@ -3731,7 +3830,7 @@
     </row>
     <row r="95" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L95" s="18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="M95" s="18">
         <f>M94/8</f>
@@ -3740,7 +3839,7 @@
     </row>
     <row r="96" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L96" s="29" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="M96" s="29">
         <f>M90*M95</f>
@@ -3778,10 +3877,10 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.35">
@@ -3790,189 +3889,189 @@
     </row>
     <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" s="15" t="s">
         <v>116</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>70</v>
-      </c>
       <c r="G4" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>86</v>
-      </c>
       <c r="F6" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>94</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>110</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>112</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I23" s="42" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I24" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -3997,13 +4096,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" t="s">
         <v>162</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>163</v>
-      </c>
-      <c r="C1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4048,10 +4147,10 @@
         <v>272</v>
       </c>
       <c r="D1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E1" t="s">
         <v>165</v>
-      </c>
-      <c r="E1" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -4074,18 +4173,18 @@
         <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -4097,4 +4196,97 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{362FEDF3-3CB3-4ABF-97BD-1ACEAE07A369}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="42" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B4" t="s">
+        <v>226</v>
+      </c>
+      <c r="C4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>230</v>
+      </c>
+      <c r="C5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C6" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>236</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Theoretically better but still not
</commit_message>
<xml_diff>
--- a/docs/Hardware.xlsx
+++ b/docs/Hardware.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\Aznable\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F768E68-CB2A-4795-853D-F2E6F25048D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5225089-5867-4D4C-A05B-5CF7609BEF7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{8387191E-7D8B-4623-897E-A5E3E75A545C}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="238">
   <si>
     <t>HEIGHT</t>
   </si>
@@ -122,9 +122,6 @@
   </si>
   <si>
     <t>UNUSED</t>
-  </si>
-  <si>
-    <t>0x0040</t>
   </si>
   <si>
     <t>Length D</t>
@@ -721,27 +718,9 @@
     <t>SPRITE_MIRROR</t>
   </si>
   <si>
-    <t>0x0020</t>
-  </si>
-  <si>
-    <t>0x0050</t>
-  </si>
-  <si>
-    <t>0x0074</t>
-  </si>
-  <si>
-    <t>0x007E</t>
-  </si>
-  <si>
-    <t>0x004E</t>
-  </si>
-  <si>
     <t>0x0004</t>
   </si>
   <si>
-    <t>0x006C</t>
-  </si>
-  <si>
     <t>Char Palette RAM</t>
   </si>
   <si>
@@ -820,7 +799,22 @@
     <t>Line RAM</t>
   </si>
   <si>
-    <t>0x2000</t>
+    <t>0x0028</t>
+  </si>
+  <si>
+    <t>0x0048</t>
+  </si>
+  <si>
+    <t>Vulcan (Vector system)</t>
+  </si>
+  <si>
+    <t>0x0200</t>
+  </si>
+  <si>
+    <t>0x00E0</t>
+  </si>
+  <si>
+    <t>0x4000</t>
   </si>
 </sst>
 </file>
@@ -1059,7 +1053,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1141,9 +1135,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1490,8 +1481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C319FCBA-55CF-4FE5-A99F-6174DD3BEDA9}">
   <dimension ref="B1:P96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B27" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1520,39 +1511,39 @@
     </row>
     <row r="2" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B2" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="F2" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="19" t="s">
-        <v>33</v>
-      </c>
       <c r="G2" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="19" t="s">
         <v>29</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>30</v>
       </c>
       <c r="J2" s="19" t="s">
         <v>24</v>
       </c>
       <c r="L2" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C3" s="22" t="s">
         <v>6</v>
@@ -1561,14 +1552,14 @@
         <v>5</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F3" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I3))</f>
         <v>0x8000</v>
       </c>
       <c r="G3" s="23">
-        <f t="shared" ref="G3:H11" si="0">HEX2DEC(MID(D3, 3, LEN(D3)-2))</f>
+        <f t="shared" ref="G3:H8" si="0">HEX2DEC(MID(D3, 3, LEN(D3)-2))</f>
         <v>0</v>
       </c>
       <c r="H3" s="23">
@@ -1576,7 +1567,7 @@
         <v>32768</v>
       </c>
       <c r="I3" s="23">
-        <f t="shared" ref="I3:I9" si="1">G3+H3</f>
+        <f t="shared" ref="I3:I7" si="1">G3+H3</f>
         <v>32768</v>
       </c>
       <c r="J3" s="23" t="s">
@@ -1595,13 +1586,13 @@
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B4" s="24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="23" t="str">
-        <f t="shared" ref="D4:D46" si="2">F3</f>
+        <f t="shared" ref="D4:D38" si="2">F3</f>
         <v>0x8000</v>
       </c>
       <c r="E4" s="23" t="s">
@@ -1668,7 +1659,7 @@
         <v>32770</v>
       </c>
       <c r="J5" s="23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L5" s="18" t="s">
         <v>0</v>
@@ -1684,64 +1675,64 @@
     <row r="6" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B6" s="24"/>
       <c r="C6" s="26"/>
-      <c r="D6" s="27" t="str">
+      <c r="D6" s="23" t="str">
         <f>F5</f>
         <v>0x8002</v>
       </c>
-      <c r="E6" s="27" t="s">
-        <v>209</v>
-      </c>
-      <c r="F6" s="27" t="str">
-        <f t="shared" ref="F6" si="6">_xlfn.CONCAT("0x",DEC2HEX(I6))</f>
-        <v>0x8080</v>
-      </c>
-      <c r="G6" s="27">
+      <c r="E6" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="F6" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I6))</f>
+        <v>0x802A</v>
+      </c>
+      <c r="G6" s="23">
         <f t="shared" si="0"/>
         <v>32770</v>
       </c>
-      <c r="H6" s="27">
+      <c r="H6" s="23">
         <f t="shared" si="0"/>
-        <v>126</v>
-      </c>
-      <c r="I6" s="27">
+        <v>40</v>
+      </c>
+      <c r="I6" s="23">
         <f t="shared" si="1"/>
-        <v>32896</v>
-      </c>
-      <c r="J6" s="27" t="s">
-        <v>26</v>
+        <v>32810</v>
+      </c>
+      <c r="J6" s="23" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B7" s="24"/>
       <c r="C7" s="26"/>
       <c r="D7" s="23" t="str">
-        <f t="shared" ref="D7" si="7">F6</f>
-        <v>0x8080</v>
+        <f>F6</f>
+        <v>0x802A</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>206</v>
+        <v>75</v>
       </c>
       <c r="F7" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I7))</f>
-        <v>0x80A0</v>
+        <v>0x803A</v>
       </c>
       <c r="G7" s="23">
-        <f t="shared" si="0"/>
-        <v>32896</v>
+        <f t="shared" ref="G7" si="6">HEX2DEC(MID(D7, 3, LEN(D7)-2))</f>
+        <v>32810</v>
       </c>
       <c r="H7" s="23">
-        <f t="shared" si="0"/>
-        <v>32</v>
+        <f t="shared" ref="H7" si="7">HEX2DEC(MID(E7, 3, LEN(E7)-2))</f>
+        <v>16</v>
       </c>
       <c r="I7" s="23">
         <f t="shared" si="1"/>
-        <v>32928</v>
+        <v>32826</v>
       </c>
       <c r="J7" s="23" t="s">
-        <v>17</v>
+        <v>203</v>
       </c>
       <c r="L7" s="20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O7" s="18">
         <f>O4*O5</f>
@@ -1749,36 +1740,39 @@
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B8" s="24"/>
+      <c r="B8" s="24">
+        <f>8*5</f>
+        <v>40</v>
+      </c>
       <c r="C8" s="26"/>
-      <c r="D8" s="27" t="str">
+      <c r="D8" s="23" t="str">
         <f>F7</f>
-        <v>0x80A0</v>
-      </c>
-      <c r="E8" s="27" t="s">
-        <v>206</v>
-      </c>
-      <c r="F8" s="27" t="str">
-        <f t="shared" ref="F8" si="8">_xlfn.CONCAT("0x",DEC2HEX(I8))</f>
-        <v>0x80C0</v>
-      </c>
-      <c r="G8" s="27">
-        <f t="shared" ref="G8:G10" si="9">HEX2DEC(MID(D8, 3, LEN(D8)-2))</f>
-        <v>32928</v>
-      </c>
-      <c r="H8" s="27">
-        <f t="shared" ref="H8:H10" si="10">HEX2DEC(MID(E8, 3, LEN(E8)-2))</f>
-        <v>32</v>
-      </c>
-      <c r="I8" s="27">
-        <f t="shared" si="1"/>
-        <v>32960</v>
-      </c>
-      <c r="J8" s="27" t="s">
-        <v>26</v>
+        <v>0x803A</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I8))</f>
+        <v>0x80FA</v>
+      </c>
+      <c r="G8" s="23">
+        <f t="shared" si="0"/>
+        <v>32826</v>
+      </c>
+      <c r="H8" s="23">
+        <f t="shared" si="0"/>
+        <v>192</v>
+      </c>
+      <c r="I8" s="23">
+        <f>G8+H8</f>
+        <v>33018</v>
+      </c>
+      <c r="J8" s="23" t="s">
+        <v>11</v>
       </c>
       <c r="L8" s="28" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M8" s="28">
         <v>256</v>
@@ -1788,33 +1782,33 @@
       <c r="B9" s="24"/>
       <c r="C9" s="26"/>
       <c r="D9" s="23" t="str">
-        <f t="shared" ref="D9" si="11">F8</f>
-        <v>0x80C0</v>
+        <f>F8</f>
+        <v>0x80FA</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>76</v>
+        <v>13</v>
       </c>
       <c r="F9" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I9))</f>
-        <v>0x80D0</v>
+        <v>0x815A</v>
       </c>
       <c r="G9" s="23">
-        <f t="shared" si="9"/>
-        <v>32960</v>
+        <f t="shared" ref="G9:H10" si="8">HEX2DEC(MID(D9, 3, LEN(D9)-2))</f>
+        <v>33018</v>
       </c>
       <c r="H9" s="23">
-        <f t="shared" si="10"/>
-        <v>16</v>
+        <f t="shared" si="8"/>
+        <v>96</v>
       </c>
       <c r="I9" s="23">
-        <f t="shared" si="1"/>
-        <v>32976</v>
+        <f>G9+H9</f>
+        <v>33114</v>
       </c>
       <c r="J9" s="23" t="s">
-        <v>204</v>
+        <v>23</v>
       </c>
       <c r="L9" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="M9" s="18">
         <v>8</v>
@@ -1823,34 +1817,34 @@
     <row r="10" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B10" s="24"/>
       <c r="C10" s="26"/>
-      <c r="D10" s="27" t="str">
+      <c r="D10" s="23" t="str">
         <f>F9</f>
-        <v>0x80D0</v>
-      </c>
-      <c r="E10" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="27" t="str">
-        <f t="shared" ref="F10" si="12">_xlfn.CONCAT("0x",DEC2HEX(I10))</f>
-        <v>0x8100</v>
-      </c>
-      <c r="G10" s="27">
-        <f t="shared" si="9"/>
-        <v>32976</v>
-      </c>
-      <c r="H10" s="27">
-        <f t="shared" si="10"/>
-        <v>48</v>
-      </c>
-      <c r="I10" s="27">
-        <f t="shared" ref="I10" si="13">G10+H10</f>
-        <v>33024</v>
-      </c>
-      <c r="J10" s="27" t="s">
-        <v>26</v>
+        <v>0x815A</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I10))</f>
+        <v>0x81BA</v>
+      </c>
+      <c r="G10" s="23">
+        <f t="shared" si="8"/>
+        <v>33114</v>
+      </c>
+      <c r="H10" s="23">
+        <f t="shared" si="8"/>
+        <v>96</v>
+      </c>
+      <c r="I10" s="23">
+        <f>G10+H10</f>
+        <v>33210</v>
+      </c>
+      <c r="J10" s="23" t="s">
+        <v>22</v>
       </c>
       <c r="L10" s="18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M10" s="18">
         <v>8</v>
@@ -1861,32 +1855,32 @@
       <c r="C11" s="26"/>
       <c r="D11" s="23" t="str">
         <f>F10</f>
-        <v>0x8100</v>
+        <v>0x81BA</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F11" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I11))</f>
-        <v>0x81C0</v>
+        <v>0x81EA</v>
       </c>
       <c r="G11" s="23">
-        <f t="shared" si="0"/>
-        <v>33024</v>
+        <f t="shared" ref="G11:H12" si="9">HEX2DEC(MID(D11, 3, LEN(D11)-2))</f>
+        <v>33210</v>
       </c>
       <c r="H11" s="23">
-        <f t="shared" si="0"/>
-        <v>192</v>
+        <f t="shared" si="9"/>
+        <v>48</v>
       </c>
       <c r="I11" s="23">
         <f>G11+H11</f>
-        <v>33216</v>
+        <v>33258</v>
       </c>
       <c r="J11" s="23" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="L11" s="18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M11" s="18">
         <v>1</v>
@@ -1895,34 +1889,34 @@
     <row r="12" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B12" s="24"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="27" t="str">
-        <f t="shared" si="2"/>
-        <v>0x81C0</v>
-      </c>
-      <c r="E12" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="27" t="str">
-        <f t="shared" ref="F12" si="14">_xlfn.CONCAT("0x",DEC2HEX(I12))</f>
-        <v>0x8200</v>
-      </c>
-      <c r="G12" s="27">
-        <f t="shared" ref="G12" si="15">HEX2DEC(MID(D12, 3, LEN(D12)-2))</f>
-        <v>33216</v>
-      </c>
-      <c r="H12" s="27">
-        <f t="shared" ref="H12" si="16">HEX2DEC(MID(E12, 3, LEN(E12)-2))</f>
-        <v>64</v>
-      </c>
-      <c r="I12" s="27">
-        <f t="shared" ref="I12" si="17">G12+H12</f>
-        <v>33280</v>
-      </c>
-      <c r="J12" s="27" t="s">
-        <v>26</v>
+      <c r="D12" s="23" t="str">
+        <f>F11</f>
+        <v>0x81EA</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I12))</f>
+        <v>0x824A</v>
+      </c>
+      <c r="G12" s="23">
+        <f t="shared" si="9"/>
+        <v>33258</v>
+      </c>
+      <c r="H12" s="23">
+        <f t="shared" si="9"/>
+        <v>96</v>
+      </c>
+      <c r="I12" s="23">
+        <f>G12+H12</f>
+        <v>33354</v>
+      </c>
+      <c r="J12" s="23" t="s">
+        <v>20</v>
       </c>
       <c r="L12" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M12" s="29">
         <f>M9*M10*M11</f>
@@ -1933,33 +1927,33 @@
       <c r="B13" s="24"/>
       <c r="C13" s="26"/>
       <c r="D13" s="23" t="str">
-        <f t="shared" si="2"/>
-        <v>0x8200</v>
+        <f>F12</f>
+        <v>0x824A</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F13" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I13))</f>
-        <v>0x8260</v>
+        <v>0x8256</v>
       </c>
       <c r="G13" s="23">
-        <f t="shared" ref="G13:H15" si="18">HEX2DEC(MID(D13, 3, LEN(D13)-2))</f>
-        <v>33280</v>
+        <f t="shared" ref="G13:H14" si="10">HEX2DEC(MID(D13, 3, LEN(D13)-2))</f>
+        <v>33354</v>
       </c>
       <c r="H13" s="23">
-        <f t="shared" si="18"/>
-        <v>96</v>
+        <f t="shared" si="10"/>
+        <v>12</v>
       </c>
       <c r="I13" s="23">
-        <f>G13+H13</f>
-        <v>33376</v>
+        <f t="shared" ref="I13:I17" si="11">G13+H13</f>
+        <v>33366</v>
       </c>
       <c r="J13" s="23" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="L13" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M13" s="18">
         <f>M12/8</f>
@@ -1969,34 +1963,34 @@
     <row r="14" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B14" s="24"/>
       <c r="C14" s="26"/>
-      <c r="D14" s="27" t="str">
-        <f t="shared" si="2"/>
-        <v>0x8260</v>
-      </c>
-      <c r="E14" s="27" t="s">
-        <v>206</v>
-      </c>
-      <c r="F14" s="27" t="str">
-        <f t="shared" ref="F14" si="19">_xlfn.CONCAT("0x",DEC2HEX(I14))</f>
-        <v>0x8280</v>
-      </c>
-      <c r="G14" s="27">
-        <f t="shared" si="18"/>
-        <v>33376</v>
-      </c>
-      <c r="H14" s="27">
-        <f t="shared" si="18"/>
-        <v>32</v>
-      </c>
-      <c r="I14" s="27">
-        <f>G14+H14</f>
-        <v>33408</v>
-      </c>
-      <c r="J14" s="27" t="s">
-        <v>26</v>
+      <c r="D14" s="23" t="str">
+        <f>F13</f>
+        <v>0x8256</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I14))</f>
+        <v>0x8286</v>
+      </c>
+      <c r="G14" s="23">
+        <f t="shared" si="10"/>
+        <v>33366</v>
+      </c>
+      <c r="H14" s="23">
+        <f t="shared" si="10"/>
+        <v>48</v>
+      </c>
+      <c r="I14" s="23">
+        <f t="shared" si="11"/>
+        <v>33414</v>
+      </c>
+      <c r="J14" s="23" t="s">
+        <v>18</v>
       </c>
       <c r="L14" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M14" s="29">
         <f>M8*M13</f>
@@ -2008,95 +2002,95 @@
       <c r="C15" s="26"/>
       <c r="D15" s="23" t="str">
         <f>F14</f>
-        <v>0x8280</v>
+        <v>0x8286</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="F15" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I15))</f>
-        <v>0x82E0</v>
+        <v>0x8296</v>
       </c>
       <c r="G15" s="23">
-        <f t="shared" si="18"/>
-        <v>33408</v>
+        <f t="shared" ref="G15:H29" si="12">HEX2DEC(MID(D15, 3, LEN(D15)-2))</f>
+        <v>33414</v>
       </c>
       <c r="H15" s="23">
-        <f t="shared" si="18"/>
-        <v>96</v>
+        <f t="shared" si="12"/>
+        <v>16</v>
       </c>
       <c r="I15" s="23">
-        <f>G15+H15</f>
-        <v>33504</v>
+        <f t="shared" si="11"/>
+        <v>33430</v>
       </c>
       <c r="J15" s="23" t="s">
-        <v>22</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B16" s="24"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="27" t="str">
-        <f t="shared" si="2"/>
-        <v>0x82E0</v>
-      </c>
-      <c r="E16" s="27" t="s">
+      <c r="C16" s="45"/>
+      <c r="D16" s="23" t="str">
+        <f t="shared" ref="D16:D22" si="13">F15</f>
+        <v>0x8296</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I16))</f>
+        <v>0x82A6</v>
+      </c>
+      <c r="G16" s="23">
+        <f t="shared" ref="G16:G17" si="14">HEX2DEC(MID(D16, 3, LEN(D16)-2))</f>
+        <v>33430</v>
+      </c>
+      <c r="H16" s="23">
+        <f t="shared" si="12"/>
+        <v>16</v>
+      </c>
+      <c r="I16" s="23">
+        <f t="shared" si="11"/>
+        <v>33446</v>
+      </c>
+      <c r="J16" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="L16" s="20" t="s">
         <v>206</v>
-      </c>
-      <c r="F16" s="27" t="str">
-        <f t="shared" ref="F16" si="20">_xlfn.CONCAT("0x",DEC2HEX(I16))</f>
-        <v>0x8300</v>
-      </c>
-      <c r="G16" s="27">
-        <f t="shared" ref="G16" si="21">HEX2DEC(MID(D16, 3, LEN(D16)-2))</f>
-        <v>33504</v>
-      </c>
-      <c r="H16" s="27">
-        <f t="shared" ref="H16" si="22">HEX2DEC(MID(E16, 3, LEN(E16)-2))</f>
-        <v>32</v>
-      </c>
-      <c r="I16" s="27">
-        <f t="shared" ref="I16" si="23">G16+H16</f>
-        <v>33536</v>
-      </c>
-      <c r="J16" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="L16" s="20" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B17" s="24"/>
-      <c r="C17" s="26"/>
+      <c r="C17" s="45"/>
       <c r="D17" s="23" t="str">
-        <f t="shared" si="2"/>
-        <v>0x8300</v>
+        <f t="shared" si="13"/>
+        <v>0x82A6</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="F17" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I17))</f>
-        <v>0x8330</v>
+        <v>0x82B6</v>
       </c>
       <c r="G17" s="23">
-        <f t="shared" ref="G17:H19" si="24">HEX2DEC(MID(D17, 3, LEN(D17)-2))</f>
-        <v>33536</v>
+        <f t="shared" si="14"/>
+        <v>33446</v>
       </c>
       <c r="H17" s="23">
-        <f t="shared" si="24"/>
-        <v>48</v>
+        <f t="shared" si="12"/>
+        <v>16</v>
       </c>
       <c r="I17" s="23">
-        <f>G17+H17</f>
-        <v>33584</v>
+        <f t="shared" si="11"/>
+        <v>33462</v>
       </c>
       <c r="J17" s="23" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="L17" s="28" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="M17" s="28">
         <v>256</v>
@@ -2109,34 +2103,34 @@
     <row r="18" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B18" s="24"/>
       <c r="C18" s="26"/>
-      <c r="D18" s="27" t="str">
-        <f t="shared" si="2"/>
-        <v>0x8330</v>
-      </c>
-      <c r="E18" s="27" t="s">
-        <v>207</v>
-      </c>
-      <c r="F18" s="27" t="str">
-        <f t="shared" ref="F18" si="25">_xlfn.CONCAT("0x",DEC2HEX(I18))</f>
-        <v>0x8380</v>
-      </c>
-      <c r="G18" s="27">
-        <f t="shared" si="24"/>
-        <v>33584</v>
-      </c>
-      <c r="H18" s="27">
-        <f t="shared" si="24"/>
-        <v>80</v>
-      </c>
-      <c r="I18" s="27">
-        <f>G18+H18</f>
-        <v>33664</v>
-      </c>
-      <c r="J18" s="27" t="s">
-        <v>26</v>
+      <c r="D18" s="23" t="str">
+        <f>F17</f>
+        <v>0x82B6</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="23" t="str">
+        <f t="shared" ref="F18" si="15">_xlfn.CONCAT("0x",DEC2HEX(I18))</f>
+        <v>0x82B7</v>
+      </c>
+      <c r="G18" s="23">
+        <f>HEX2DEC(MID(D18, 3, LEN(D18)-2))</f>
+        <v>33462</v>
+      </c>
+      <c r="H18" s="23">
+        <f t="shared" ref="H18" si="16">HEX2DEC(MID(E18, 3, LEN(E18)-2))</f>
+        <v>1</v>
+      </c>
+      <c r="I18" s="23">
+        <f t="shared" ref="I18" si="17">G18+H18</f>
+        <v>33463</v>
+      </c>
+      <c r="J18" s="23" t="s">
+        <v>155</v>
       </c>
       <c r="L18" s="18" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="M18" s="18">
         <v>32</v>
@@ -2147,32 +2141,32 @@
       <c r="C19" s="26"/>
       <c r="D19" s="23" t="str">
         <f>F18</f>
-        <v>0x8380</v>
+        <v>0x82B7</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F19" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I19))</f>
-        <v>0x83E0</v>
+        <f t="shared" ref="F19" si="18">_xlfn.CONCAT("0x",DEC2HEX(I19))</f>
+        <v>0x82B8</v>
       </c>
       <c r="G19" s="23">
-        <f t="shared" si="24"/>
-        <v>33664</v>
+        <f>HEX2DEC(MID(D19, 3, LEN(D19)-2))</f>
+        <v>33463</v>
       </c>
       <c r="H19" s="23">
-        <f t="shared" si="24"/>
-        <v>96</v>
+        <f t="shared" ref="H19" si="19">HEX2DEC(MID(E19, 3, LEN(E19)-2))</f>
+        <v>1</v>
       </c>
       <c r="I19" s="23">
-        <f>G19+H19</f>
-        <v>33760</v>
+        <f t="shared" ref="I19" si="20">G19+H19</f>
+        <v>33464</v>
       </c>
       <c r="J19" s="23" t="s">
-        <v>20</v>
+        <v>201</v>
       </c>
       <c r="L19" s="29" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="M19" s="29">
         <f>M18</f>
@@ -2181,35 +2175,35 @@
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B20" s="24"/>
-      <c r="C20" s="26"/>
+      <c r="C20" s="27"/>
       <c r="D20" s="27" t="str">
-        <f t="shared" si="2"/>
-        <v>0x83E0</v>
+        <f>F19</f>
+        <v>0x82B8</v>
       </c>
       <c r="E20" s="27" t="s">
-        <v>206</v>
+        <v>233</v>
       </c>
       <c r="F20" s="27" t="str">
-        <f t="shared" ref="F20" si="26">_xlfn.CONCAT("0x",DEC2HEX(I20))</f>
-        <v>0x8400</v>
+        <f t="shared" ref="F20" si="21">_xlfn.CONCAT("0x",DEC2HEX(I20))</f>
+        <v>0x8300</v>
       </c>
       <c r="G20" s="27">
-        <f t="shared" ref="G20" si="27">HEX2DEC(MID(D20, 3, LEN(D20)-2))</f>
-        <v>33760</v>
+        <f>HEX2DEC(MID(D20, 3, LEN(D20)-2))</f>
+        <v>33464</v>
       </c>
       <c r="H20" s="27">
-        <f t="shared" ref="H20" si="28">HEX2DEC(MID(E20, 3, LEN(E20)-2))</f>
-        <v>32</v>
+        <f t="shared" ref="H20" si="22">HEX2DEC(MID(E20, 3, LEN(E20)-2))</f>
+        <v>72</v>
       </c>
       <c r="I20" s="27">
-        <f t="shared" ref="I20" si="29">G20+H20</f>
-        <v>33792</v>
+        <f t="shared" ref="I20" si="23">G20+H20</f>
+        <v>33536</v>
       </c>
       <c r="J20" s="27" t="s">
         <v>26</v>
       </c>
       <c r="L20" s="18" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="M20" s="18">
         <f>M19/8</f>
@@ -2218,35 +2212,37 @@
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B21" s="24"/>
-      <c r="C21" s="26"/>
+      <c r="C21" s="46" t="s">
+        <v>144</v>
+      </c>
       <c r="D21" s="23" t="str">
-        <f t="shared" si="2"/>
-        <v>0x8400</v>
+        <f>F20</f>
+        <v>0x8300</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="F21" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I21))</f>
-        <v>0x840C</v>
+        <v>0x8310</v>
       </c>
       <c r="G21" s="23">
-        <f t="shared" ref="G21:H23" si="30">HEX2DEC(MID(D21, 3, LEN(D21)-2))</f>
-        <v>33792</v>
+        <f t="shared" ref="G21" si="24">HEX2DEC(MID(D21, 3, LEN(D21)-2))</f>
+        <v>33536</v>
       </c>
       <c r="H21" s="23">
-        <f t="shared" si="30"/>
-        <v>12</v>
+        <f t="shared" si="12"/>
+        <v>16</v>
       </c>
       <c r="I21" s="23">
-        <f t="shared" ref="I21:I27" si="31">G21+H21</f>
-        <v>33804</v>
+        <f>G21+H21</f>
+        <v>33552</v>
       </c>
       <c r="J21" s="23" t="s">
-        <v>19</v>
+        <v>158</v>
       </c>
       <c r="L21" s="29" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="M21" s="29">
         <f>M17*M20</f>
@@ -2255,98 +2251,100 @@
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B22" s="24"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="27" t="str">
-        <f t="shared" si="2"/>
-        <v>0x840C</v>
-      </c>
-      <c r="E22" s="27" t="s">
-        <v>208</v>
-      </c>
-      <c r="F22" s="27" t="str">
-        <f t="shared" ref="F22" si="32">_xlfn.CONCAT("0x",DEC2HEX(I22))</f>
-        <v>0x8480</v>
-      </c>
-      <c r="G22" s="27">
-        <f t="shared" si="30"/>
-        <v>33804</v>
-      </c>
-      <c r="H22" s="27">
-        <f t="shared" si="30"/>
-        <v>116</v>
-      </c>
-      <c r="I22" s="27">
-        <f t="shared" si="31"/>
-        <v>33920</v>
-      </c>
-      <c r="J22" s="27" t="s">
-        <v>26</v>
+      <c r="C22" s="45"/>
+      <c r="D22" s="23" t="str">
+        <f t="shared" si="13"/>
+        <v>0x8310</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>205</v>
+      </c>
+      <c r="F22" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I22))</f>
+        <v>0x8314</v>
+      </c>
+      <c r="G22" s="23">
+        <f t="shared" ref="G22:G24" si="25">HEX2DEC(MID(D22, 3, LEN(D22)-2))</f>
+        <v>33552</v>
+      </c>
+      <c r="H22" s="23">
+        <f t="shared" ref="H22:H24" si="26">HEX2DEC(MID(E22, 3, LEN(E22)-2))</f>
+        <v>4</v>
+      </c>
+      <c r="I22" s="23">
+        <f>G22+H22</f>
+        <v>33556</v>
+      </c>
+      <c r="J22" s="23" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B23" s="24"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="23" t="str">
-        <f t="shared" si="2"/>
-        <v>0x8480</v>
-      </c>
-      <c r="E23" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I23))</f>
-        <v>0x84B0</v>
-      </c>
-      <c r="G23" s="23">
-        <f t="shared" si="30"/>
-        <v>33920</v>
-      </c>
-      <c r="H23" s="23">
-        <f t="shared" si="30"/>
-        <v>48</v>
-      </c>
-      <c r="I23" s="23">
-        <f t="shared" si="31"/>
-        <v>33968</v>
-      </c>
-      <c r="J23" s="23" t="s">
-        <v>18</v>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27" t="str">
+        <f>F22</f>
+        <v>0x8314</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="27" t="str">
+        <f t="shared" ref="F23" si="27">_xlfn.CONCAT("0x",DEC2HEX(I23))</f>
+        <v>0x8320</v>
+      </c>
+      <c r="G23" s="27">
+        <f t="shared" si="25"/>
+        <v>33556</v>
+      </c>
+      <c r="H23" s="27">
+        <f t="shared" si="26"/>
+        <v>12</v>
+      </c>
+      <c r="I23" s="27">
+        <f t="shared" ref="I23" si="28">G23+H23</f>
+        <v>33568</v>
+      </c>
+      <c r="J23" s="27" t="s">
+        <v>26</v>
       </c>
       <c r="L23" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B24" s="24"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="27" t="str">
+      <c r="C24" s="43" t="s">
+        <v>234</v>
+      </c>
+      <c r="D24" s="23" t="str">
         <f>F23</f>
-        <v>0x84B0</v>
-      </c>
-      <c r="E24" s="27" t="s">
-        <v>207</v>
-      </c>
-      <c r="F24" s="27" t="str">
-        <f t="shared" ref="F24" si="33">_xlfn.CONCAT("0x",DEC2HEX(I24))</f>
-        <v>0x8500</v>
-      </c>
-      <c r="G24" s="27">
-        <f t="shared" ref="G24:H37" si="34">HEX2DEC(MID(D24, 3, LEN(D24)-2))</f>
-        <v>33968</v>
-      </c>
-      <c r="H24" s="27">
-        <f t="shared" si="34"/>
-        <v>80</v>
-      </c>
-      <c r="I24" s="27">
-        <f t="shared" si="31"/>
-        <v>34048</v>
-      </c>
-      <c r="J24" s="27" t="s">
-        <v>26</v>
+        <v>0x8320</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>235</v>
+      </c>
+      <c r="F24" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I24))</f>
+        <v>0x8520</v>
+      </c>
+      <c r="G24" s="23">
+        <f t="shared" si="25"/>
+        <v>33568</v>
+      </c>
+      <c r="H24" s="23">
+        <f t="shared" si="26"/>
+        <v>512</v>
+      </c>
+      <c r="I24" s="23">
+        <f>G24+H24</f>
+        <v>34080</v>
+      </c>
+      <c r="J24" s="23" t="s">
+        <v>175</v>
       </c>
       <c r="L24" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M24" s="28">
         <v>4</v>
@@ -2354,74 +2352,77 @@
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B25" s="24"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="23" t="str">
+      <c r="C25" s="27"/>
+      <c r="D25" s="27" t="str">
         <f>F24</f>
-        <v>0x8500</v>
-      </c>
-      <c r="E25" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="F25" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I25))</f>
-        <v>0x8510</v>
-      </c>
-      <c r="G25" s="23">
-        <f t="shared" si="34"/>
-        <v>34048</v>
-      </c>
-      <c r="H25" s="23">
-        <f t="shared" si="34"/>
-        <v>16</v>
-      </c>
-      <c r="I25" s="23">
-        <f t="shared" si="31"/>
-        <v>34064</v>
-      </c>
-      <c r="J25" s="23" t="s">
-        <v>79</v>
+        <v>0x8520</v>
+      </c>
+      <c r="E25" s="27" t="s">
+        <v>236</v>
+      </c>
+      <c r="F25" s="27" t="str">
+        <f t="shared" ref="F25" si="29">_xlfn.CONCAT("0x",DEC2HEX(I25))</f>
+        <v>0x8600</v>
+      </c>
+      <c r="G25" s="27">
+        <f t="shared" ref="G25:G27" si="30">HEX2DEC(MID(D25, 3, LEN(D25)-2))</f>
+        <v>34080</v>
+      </c>
+      <c r="H25" s="27">
+        <f t="shared" ref="H25:H28" si="31">HEX2DEC(MID(E25, 3, LEN(E25)-2))</f>
+        <v>224</v>
+      </c>
+      <c r="I25" s="27">
+        <f t="shared" ref="I25" si="32">G25+H25</f>
+        <v>34304</v>
+      </c>
+      <c r="J25" s="27" t="s">
+        <v>26</v>
       </c>
       <c r="L25" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M25" s="18">
         <v>16</v>
       </c>
       <c r="N25" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B26" s="24"/>
-      <c r="C26" s="46"/>
+      <c r="C26" s="43" t="s">
+        <v>173</v>
+      </c>
       <c r="D26" s="23" t="str">
-        <f t="shared" ref="D26:D32" si="35">F25</f>
-        <v>0x8510</v>
-      </c>
-      <c r="E26" s="23" t="s">
-        <v>76</v>
+        <f>F25</f>
+        <v>0x8600</v>
+      </c>
+      <c r="E26" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M80))</f>
+        <v>0x10</v>
       </c>
       <c r="F26" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I26))</f>
-        <v>0x8520</v>
+        <v>0x8610</v>
       </c>
       <c r="G26" s="23">
-        <f t="shared" ref="G26:G27" si="36">HEX2DEC(MID(D26, 3, LEN(D26)-2))</f>
-        <v>34064</v>
+        <f t="shared" ref="G26" si="33">HEX2DEC(MID(D26, 3, LEN(D26)-2))</f>
+        <v>34304</v>
       </c>
       <c r="H26" s="23">
-        <f t="shared" si="34"/>
+        <f t="shared" si="31"/>
         <v>16</v>
       </c>
       <c r="I26" s="23">
-        <f t="shared" si="31"/>
-        <v>34080</v>
+        <f>G26+H26</f>
+        <v>34320</v>
       </c>
       <c r="J26" s="23" t="s">
-        <v>77</v>
+        <v>175</v>
       </c>
       <c r="L26" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M26" s="18">
         <v>32</v>
@@ -2429,35 +2430,36 @@
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B27" s="24"/>
-      <c r="C27" s="46"/>
+      <c r="C27" s="44"/>
       <c r="D27" s="23" t="str">
-        <f t="shared" si="35"/>
-        <v>0x8520</v>
-      </c>
-      <c r="E27" s="23" t="s">
-        <v>76</v>
+        <f>F26</f>
+        <v>0x8610</v>
+      </c>
+      <c r="E27" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M87))</f>
+        <v>0x300</v>
       </c>
       <c r="F27" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I27))</f>
-        <v>0x8530</v>
+        <v>0x8910</v>
       </c>
       <c r="G27" s="23">
-        <f t="shared" si="36"/>
-        <v>34080</v>
+        <f t="shared" si="30"/>
+        <v>34320</v>
       </c>
       <c r="H27" s="23">
-        <f t="shared" si="34"/>
-        <v>16</v>
+        <f t="shared" si="31"/>
+        <v>768</v>
       </c>
       <c r="I27" s="23">
-        <f t="shared" si="31"/>
-        <v>34096</v>
+        <f>G27+H27</f>
+        <v>35088</v>
       </c>
       <c r="J27" s="23" t="s">
-        <v>78</v>
+        <v>180</v>
       </c>
       <c r="L27" s="29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M27" s="29">
         <f>M25*M26</f>
@@ -2466,35 +2468,35 @@
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B28" s="24"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="23" t="str">
+      <c r="C28" s="27"/>
+      <c r="D28" s="27" t="str">
         <f>F27</f>
-        <v>0x8530</v>
-      </c>
-      <c r="E28" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="23" t="str">
-        <f t="shared" ref="F28" si="37">_xlfn.CONCAT("0x",DEC2HEX(I28))</f>
-        <v>0x8531</v>
-      </c>
-      <c r="G28" s="23">
-        <f>HEX2DEC(MID(D28, 3, LEN(D28)-2))</f>
-        <v>34096</v>
-      </c>
-      <c r="H28" s="23">
-        <f t="shared" ref="H28" si="38">HEX2DEC(MID(E28, 3, LEN(E28)-2))</f>
-        <v>1</v>
-      </c>
-      <c r="I28" s="23">
-        <f t="shared" ref="I28" si="39">G28+H28</f>
-        <v>34097</v>
-      </c>
-      <c r="J28" s="23" t="s">
-        <v>156</v>
+        <v>0x8910</v>
+      </c>
+      <c r="E28" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="F28" s="27" t="str">
+        <f t="shared" ref="F28" si="34">_xlfn.CONCAT("0x",DEC2HEX(I28))</f>
+        <v>0x8A00</v>
+      </c>
+      <c r="G28" s="27">
+        <f t="shared" ref="G28" si="35">HEX2DEC(MID(D28, 3, LEN(D28)-2))</f>
+        <v>35088</v>
+      </c>
+      <c r="H28" s="27">
+        <f t="shared" si="31"/>
+        <v>240</v>
+      </c>
+      <c r="I28" s="27">
+        <f t="shared" ref="I28" si="36">G28+H28</f>
+        <v>35328</v>
+      </c>
+      <c r="J28" s="27" t="s">
+        <v>26</v>
       </c>
       <c r="L28" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M28" s="18">
         <f>M27/8</f>
@@ -2503,35 +2505,37 @@
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B29" s="24"/>
-      <c r="C29" s="26"/>
+      <c r="C29" s="30" t="s">
+        <v>38</v>
+      </c>
       <c r="D29" s="23" t="str">
         <f>F28</f>
-        <v>0x8531</v>
+        <v>0x8A00</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F29" s="23" t="str">
-        <f t="shared" ref="F29" si="40">_xlfn.CONCAT("0x",DEC2HEX(I29))</f>
-        <v>0x8532</v>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I29))</f>
+        <v>0x9200</v>
       </c>
       <c r="G29" s="23">
         <f>HEX2DEC(MID(D29, 3, LEN(D29)-2))</f>
-        <v>34097</v>
+        <v>35328</v>
       </c>
       <c r="H29" s="23">
-        <f t="shared" ref="H29" si="41">HEX2DEC(MID(E29, 3, LEN(E29)-2))</f>
-        <v>1</v>
+        <f t="shared" si="12"/>
+        <v>2048</v>
       </c>
       <c r="I29" s="23">
-        <f t="shared" ref="I29" si="42">G29+H29</f>
-        <v>34098</v>
+        <f>G29+H29</f>
+        <v>37376</v>
       </c>
       <c r="J29" s="23" t="s">
-        <v>202</v>
+        <v>8</v>
       </c>
       <c r="L29" s="29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M29" s="29">
         <f>M28*M24</f>
@@ -2540,103 +2544,101 @@
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B30" s="24"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27" t="str">
-        <f>F29</f>
-        <v>0x8532</v>
-      </c>
-      <c r="E30" s="27" t="s">
-        <v>210</v>
-      </c>
-      <c r="F30" s="27" t="str">
-        <f t="shared" ref="F30" si="43">_xlfn.CONCAT("0x",DEC2HEX(I30))</f>
-        <v>0x8580</v>
-      </c>
-      <c r="G30" s="27">
+      <c r="C30" s="31"/>
+      <c r="D30" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>0x9200</v>
+      </c>
+      <c r="E30" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I30))</f>
+        <v>0x9A00</v>
+      </c>
+      <c r="G30" s="23">
         <f>HEX2DEC(MID(D30, 3, LEN(D30)-2))</f>
-        <v>34098</v>
-      </c>
-      <c r="H30" s="27">
-        <f t="shared" ref="H30" si="44">HEX2DEC(MID(E30, 3, LEN(E30)-2))</f>
-        <v>78</v>
-      </c>
-      <c r="I30" s="27">
-        <f t="shared" ref="I30" si="45">G30+H30</f>
-        <v>34176</v>
-      </c>
-      <c r="J30" s="27" t="s">
-        <v>26</v>
+        <v>37376</v>
+      </c>
+      <c r="H30" s="23">
+        <f>HEX2DEC(MID(E30, 3, LEN(E30)-2))</f>
+        <v>2048</v>
+      </c>
+      <c r="I30" s="23">
+        <f>G30+H30</f>
+        <v>39424</v>
+      </c>
+      <c r="J30" s="23" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B31" s="24"/>
-      <c r="C31" s="47" t="s">
-        <v>145</v>
-      </c>
+      <c r="C31" s="31"/>
       <c r="D31" s="23" t="str">
-        <f>F30</f>
-        <v>0x8580</v>
+        <f t="shared" si="2"/>
+        <v>0x9A00</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="F31" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I31))</f>
-        <v>0x8590</v>
+        <f t="shared" ref="F31" si="37">_xlfn.CONCAT("0x",DEC2HEX(I31))</f>
+        <v>0xA200</v>
       </c>
       <c r="G31" s="23">
-        <f t="shared" ref="G31" si="46">HEX2DEC(MID(D31, 3, LEN(D31)-2))</f>
-        <v>34176</v>
+        <f t="shared" ref="G31" si="38">HEX2DEC(MID(D31, 3, LEN(D31)-2))</f>
+        <v>39424</v>
       </c>
       <c r="H31" s="23">
-        <f t="shared" si="34"/>
-        <v>16</v>
+        <f t="shared" ref="H31" si="39">HEX2DEC(MID(E31, 3, LEN(E31)-2))</f>
+        <v>2048</v>
       </c>
       <c r="I31" s="23">
-        <f>G31+H31</f>
-        <v>34192</v>
+        <f t="shared" ref="I31" si="40">G31+H31</f>
+        <v>41472</v>
       </c>
       <c r="J31" s="23" t="s">
-        <v>159</v>
+        <v>35</v>
       </c>
       <c r="L31" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N31" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B32" s="24"/>
-      <c r="C32" s="46"/>
+      <c r="C32" s="31"/>
       <c r="D32" s="23" t="str">
-        <f t="shared" si="35"/>
-        <v>0x8590</v>
+        <f t="shared" si="2"/>
+        <v>0xA200</v>
       </c>
       <c r="E32" s="23" t="s">
-        <v>211</v>
+        <v>7</v>
       </c>
       <c r="F32" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I32))</f>
-        <v>0x8594</v>
+        <f t="shared" ref="F32:F36" si="41">_xlfn.CONCAT("0x",DEC2HEX(I32))</f>
+        <v>0xAA00</v>
       </c>
       <c r="G32" s="23">
-        <f t="shared" ref="G32" si="47">HEX2DEC(MID(D32, 3, LEN(D32)-2))</f>
-        <v>34192</v>
+        <f t="shared" ref="G32:G36" si="42">HEX2DEC(MID(D32, 3, LEN(D32)-2))</f>
+        <v>41472</v>
       </c>
       <c r="H32" s="23">
-        <f t="shared" ref="H32" si="48">HEX2DEC(MID(E32, 3, LEN(E32)-2))</f>
-        <v>4</v>
+        <f t="shared" ref="H32:H36" si="43">HEX2DEC(MID(E32, 3, LEN(E32)-2))</f>
+        <v>2048</v>
       </c>
       <c r="I32" s="23">
-        <f>G32+H32</f>
-        <v>34196</v>
+        <f t="shared" ref="I32:I36" si="44">G32+H32</f>
+        <v>43520</v>
       </c>
       <c r="J32" s="23" t="s">
-        <v>160</v>
+        <v>37</v>
       </c>
       <c r="L32" s="28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M32" s="28">
         <v>64</v>
@@ -2644,35 +2646,35 @@
     </row>
     <row r="33" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="24"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27" t="str">
+      <c r="C33" s="31"/>
+      <c r="D33" s="23" t="str">
         <f>F32</f>
-        <v>0x8594</v>
-      </c>
-      <c r="E33" s="27" t="s">
+        <v>0xAA00</v>
+      </c>
+      <c r="E33" s="23" t="s">
         <v>212</v>
       </c>
-      <c r="F33" s="27" t="str">
-        <f t="shared" ref="F33" si="49">_xlfn.CONCAT("0x",DEC2HEX(I33))</f>
-        <v>0x8600</v>
-      </c>
-      <c r="G33" s="27">
-        <f t="shared" ref="G33:G35" si="50">HEX2DEC(MID(D33, 3, LEN(D33)-2))</f>
-        <v>34196</v>
-      </c>
-      <c r="H33" s="27">
-        <f t="shared" ref="H33:H36" si="51">HEX2DEC(MID(E33, 3, LEN(E33)-2))</f>
-        <v>108</v>
-      </c>
-      <c r="I33" s="27">
-        <f t="shared" ref="I33" si="52">G33+H33</f>
-        <v>34304</v>
-      </c>
-      <c r="J33" s="27" t="s">
-        <v>26</v>
+      <c r="F33" s="23" t="str">
+        <f t="shared" ref="F33" si="45">_xlfn.CONCAT("0x",DEC2HEX(I33))</f>
+        <v>0xAB00</v>
+      </c>
+      <c r="G33" s="23">
+        <f t="shared" ref="G33" si="46">HEX2DEC(MID(D33, 3, LEN(D33)-2))</f>
+        <v>43520</v>
+      </c>
+      <c r="H33" s="23">
+        <f t="shared" ref="H33" si="47">HEX2DEC(MID(E33, 3, LEN(E33)-2))</f>
+        <v>256</v>
+      </c>
+      <c r="I33" s="23">
+        <f t="shared" ref="I33" si="48">G33+H33</f>
+        <v>43776</v>
+      </c>
+      <c r="J33" s="23" t="s">
+        <v>214</v>
       </c>
       <c r="L33" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M33" s="18">
         <v>16</v>
@@ -2680,38 +2682,35 @@
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B34" s="24"/>
-      <c r="C34" s="44" t="s">
-        <v>174</v>
-      </c>
+      <c r="C34" s="31"/>
       <c r="D34" s="23" t="str">
         <f>F33</f>
-        <v>0x8600</v>
-      </c>
-      <c r="E34" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M80))</f>
-        <v>0x10</v>
+        <v>0xAB00</v>
+      </c>
+      <c r="E34" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="F34" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I34))</f>
-        <v>0x8610</v>
+        <f t="shared" si="41"/>
+        <v>0xAC00</v>
       </c>
       <c r="G34" s="23">
-        <f t="shared" ref="G34" si="53">HEX2DEC(MID(D34, 3, LEN(D34)-2))</f>
-        <v>34304</v>
+        <f t="shared" si="42"/>
+        <v>43776</v>
       </c>
       <c r="H34" s="23">
-        <f t="shared" si="51"/>
-        <v>16</v>
+        <f t="shared" si="43"/>
+        <v>256</v>
       </c>
       <c r="I34" s="23">
-        <f>G34+H34</f>
-        <v>34320</v>
+        <f t="shared" si="44"/>
+        <v>44032</v>
       </c>
       <c r="J34" s="23" t="s">
-        <v>176</v>
+        <v>215</v>
       </c>
       <c r="L34" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M34" s="18">
         <v>16</v>
@@ -2719,42 +2718,41 @@
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B35" s="24"/>
-      <c r="C35" s="45"/>
+      <c r="C35" s="32"/>
       <c r="D35" s="23" t="str">
         <f>F34</f>
-        <v>0x8610</v>
-      </c>
-      <c r="E35" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M87))</f>
-        <v>0x300</v>
+        <v>0xAC00</v>
+      </c>
+      <c r="E35" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="F35" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I35))</f>
-        <v>0x8910</v>
+        <f t="shared" ref="F35" si="49">_xlfn.CONCAT("0x",DEC2HEX(I35))</f>
+        <v>0xAD00</v>
       </c>
       <c r="G35" s="23">
-        <f t="shared" si="50"/>
-        <v>34320</v>
+        <f t="shared" ref="G35" si="50">HEX2DEC(MID(D35, 3, LEN(D35)-2))</f>
+        <v>44032</v>
       </c>
       <c r="H35" s="23">
-        <f t="shared" si="51"/>
-        <v>768</v>
+        <f t="shared" ref="H35" si="51">HEX2DEC(MID(E35, 3, LEN(E35)-2))</f>
+        <v>256</v>
       </c>
       <c r="I35" s="23">
-        <f>G35+H35</f>
-        <v>35088</v>
+        <f t="shared" ref="I35" si="52">G35+H35</f>
+        <v>44288</v>
       </c>
       <c r="J35" s="23" t="s">
-        <v>181</v>
+        <v>216</v>
       </c>
       <c r="L35" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M35" s="18">
         <v>8</v>
       </c>
       <c r="N35" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.2">
@@ -2762,32 +2760,32 @@
       <c r="C36" s="27"/>
       <c r="D36" s="27" t="str">
         <f>F35</f>
-        <v>0x8910</v>
+        <v>0xAD00</v>
       </c>
       <c r="E36" s="27" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="F36" s="27" t="str">
-        <f t="shared" ref="F36" si="54">_xlfn.CONCAT("0x",DEC2HEX(I36))</f>
-        <v>0x8A00</v>
+        <f t="shared" si="41"/>
+        <v>0xB000</v>
       </c>
       <c r="G36" s="27">
-        <f t="shared" ref="G36" si="55">HEX2DEC(MID(D36, 3, LEN(D36)-2))</f>
-        <v>35088</v>
+        <f t="shared" si="42"/>
+        <v>44288</v>
       </c>
       <c r="H36" s="27">
-        <f t="shared" si="51"/>
-        <v>240</v>
+        <f t="shared" si="43"/>
+        <v>768</v>
       </c>
       <c r="I36" s="27">
-        <f t="shared" ref="I36" si="56">G36+H36</f>
-        <v>35328</v>
+        <f t="shared" si="44"/>
+        <v>45056</v>
       </c>
       <c r="J36" s="27" t="s">
         <v>26</v>
       </c>
       <c r="L36" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M36" s="29">
         <f>M33*M34*M35</f>
@@ -2796,37 +2794,38 @@
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B37" s="24"/>
-      <c r="C37" s="30" t="s">
-        <v>39</v>
+      <c r="C37" s="33" t="s">
+        <v>46</v>
       </c>
       <c r="D37" s="23" t="str">
         <f>F36</f>
-        <v>0x8A00</v>
-      </c>
-      <c r="E37" s="23" t="s">
-        <v>7</v>
+        <v>0xB000</v>
+      </c>
+      <c r="E37" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M52))</f>
+        <v>0x80</v>
       </c>
       <c r="F37" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I37))</f>
-        <v>0x9200</v>
+        <f t="shared" ref="F37:F38" si="53">_xlfn.CONCAT("0x",DEC2HEX(I37))</f>
+        <v>0xB080</v>
       </c>
       <c r="G37" s="23">
-        <f>HEX2DEC(MID(D37, 3, LEN(D37)-2))</f>
-        <v>35328</v>
+        <f t="shared" ref="G37:G38" si="54">HEX2DEC(MID(D37, 3, LEN(D37)-2))</f>
+        <v>45056</v>
       </c>
       <c r="H37" s="23">
-        <f t="shared" si="34"/>
-        <v>2048</v>
+        <f t="shared" ref="H37:H38" si="55">HEX2DEC(MID(E37, 3, LEN(E37)-2))</f>
+        <v>128</v>
       </c>
       <c r="I37" s="23">
-        <f>G37+H37</f>
-        <v>37376</v>
+        <f t="shared" ref="I37:I38" si="56">G37+H37</f>
+        <v>45184</v>
       </c>
       <c r="J37" s="23" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="L37" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M37" s="18">
         <f>M36/8</f>
@@ -2835,35 +2834,35 @@
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B38" s="24"/>
-      <c r="C38" s="31"/>
-      <c r="D38" s="23" t="str">
+      <c r="C38" s="34"/>
+      <c r="D38" s="27" t="str">
         <f t="shared" si="2"/>
-        <v>0x9200</v>
-      </c>
-      <c r="E38" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="F38" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I38))</f>
-        <v>0x9A00</v>
-      </c>
-      <c r="G38" s="23">
-        <f>HEX2DEC(MID(D38, 3, LEN(D38)-2))</f>
-        <v>37376</v>
-      </c>
-      <c r="H38" s="23">
-        <f>HEX2DEC(MID(E38, 3, LEN(E38)-2))</f>
-        <v>2048</v>
-      </c>
-      <c r="I38" s="23">
-        <f>G38+H38</f>
-        <v>39424</v>
-      </c>
-      <c r="J38" s="23" t="s">
-        <v>37</v>
+        <v>0xB080</v>
+      </c>
+      <c r="E38" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="F38" s="27" t="str">
+        <f t="shared" si="53"/>
+        <v>0xB400</v>
+      </c>
+      <c r="G38" s="27">
+        <f t="shared" si="54"/>
+        <v>45184</v>
+      </c>
+      <c r="H38" s="27">
+        <f t="shared" si="55"/>
+        <v>896</v>
+      </c>
+      <c r="I38" s="27">
+        <f t="shared" si="56"/>
+        <v>46080</v>
+      </c>
+      <c r="J38" s="27" t="s">
+        <v>26</v>
       </c>
       <c r="L38" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M38" s="29">
         <f>M32*M37</f>
@@ -2872,98 +2871,100 @@
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B39" s="24"/>
-      <c r="C39" s="31"/>
+      <c r="C39" s="34"/>
       <c r="D39" s="23" t="str">
-        <f t="shared" si="2"/>
-        <v>0x9A00</v>
-      </c>
-      <c r="E39" s="23" t="s">
-        <v>7</v>
+        <f t="shared" ref="D39:D40" si="57">F38</f>
+        <v>0xB400</v>
+      </c>
+      <c r="E39" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M65))</f>
+        <v>0x4</v>
       </c>
       <c r="F39" s="23" t="str">
-        <f t="shared" ref="F39" si="57">_xlfn.CONCAT("0x",DEC2HEX(I39))</f>
-        <v>0xA200</v>
+        <f t="shared" ref="F39:F40" si="58">_xlfn.CONCAT("0x",DEC2HEX(I39))</f>
+        <v>0xB404</v>
       </c>
       <c r="G39" s="23">
-        <f t="shared" ref="G39" si="58">HEX2DEC(MID(D39, 3, LEN(D39)-2))</f>
-        <v>39424</v>
+        <f t="shared" ref="G39:G40" si="59">HEX2DEC(MID(D39, 3, LEN(D39)-2))</f>
+        <v>46080</v>
       </c>
       <c r="H39" s="23">
-        <f t="shared" ref="H39" si="59">HEX2DEC(MID(E39, 3, LEN(E39)-2))</f>
-        <v>2048</v>
+        <f t="shared" ref="H39:H40" si="60">HEX2DEC(MID(E39, 3, LEN(E39)-2))</f>
+        <v>4</v>
       </c>
       <c r="I39" s="23">
-        <f t="shared" ref="I39" si="60">G39+H39</f>
-        <v>41472</v>
+        <f t="shared" ref="I39:I40" si="61">G39+H39</f>
+        <v>46084</v>
       </c>
       <c r="J39" s="23" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B40" s="24"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="23" t="str">
-        <f t="shared" si="2"/>
-        <v>0xA200</v>
-      </c>
-      <c r="E40" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="F40" s="23" t="str">
-        <f t="shared" ref="F40:F44" si="61">_xlfn.CONCAT("0x",DEC2HEX(I40))</f>
-        <v>0xAA00</v>
-      </c>
-      <c r="G40" s="23">
-        <f t="shared" ref="G40:G44" si="62">HEX2DEC(MID(D40, 3, LEN(D40)-2))</f>
-        <v>41472</v>
-      </c>
-      <c r="H40" s="23">
-        <f t="shared" ref="H40:H44" si="63">HEX2DEC(MID(E40, 3, LEN(E40)-2))</f>
-        <v>2048</v>
-      </c>
-      <c r="I40" s="23">
-        <f t="shared" ref="I40:I44" si="64">G40+H40</f>
-        <v>43520</v>
-      </c>
-      <c r="J40" s="23" t="s">
-        <v>38</v>
+      <c r="C40" s="34"/>
+      <c r="D40" s="27" t="str">
+        <f t="shared" si="57"/>
+        <v>0xB404</v>
+      </c>
+      <c r="E40" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="F40" s="27" t="str">
+        <f t="shared" si="58"/>
+        <v>0xB800</v>
+      </c>
+      <c r="G40" s="27">
+        <f t="shared" si="59"/>
+        <v>46084</v>
+      </c>
+      <c r="H40" s="27">
+        <f t="shared" si="60"/>
+        <v>1020</v>
+      </c>
+      <c r="I40" s="27">
+        <f t="shared" si="61"/>
+        <v>47104</v>
+      </c>
+      <c r="J40" s="27" t="s">
+        <v>26</v>
       </c>
       <c r="L40" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B41" s="24"/>
-      <c r="C41" s="31"/>
+      <c r="C41" s="35"/>
       <c r="D41" s="23" t="str">
         <f>F40</f>
-        <v>0xAA00</v>
-      </c>
-      <c r="E41" s="23" t="s">
-        <v>219</v>
+        <v>0xB800</v>
+      </c>
+      <c r="E41" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M59))</f>
+        <v>0x800</v>
       </c>
       <c r="F41" s="23" t="str">
-        <f t="shared" ref="F41" si="65">_xlfn.CONCAT("0x",DEC2HEX(I41))</f>
-        <v>0xAB00</v>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I41))</f>
+        <v>0xC000</v>
       </c>
       <c r="G41" s="23">
-        <f t="shared" ref="G41" si="66">HEX2DEC(MID(D41, 3, LEN(D41)-2))</f>
-        <v>43520</v>
+        <f t="shared" ref="G41:H42" si="62">HEX2DEC(MID(D41, 3, LEN(D41)-2))</f>
+        <v>47104</v>
       </c>
       <c r="H41" s="23">
-        <f t="shared" ref="H41" si="67">HEX2DEC(MID(E41, 3, LEN(E41)-2))</f>
-        <v>256</v>
+        <f t="shared" si="62"/>
+        <v>2048</v>
       </c>
       <c r="I41" s="23">
-        <f t="shared" ref="I41" si="68">G41+H41</f>
-        <v>43776</v>
+        <f>G41+H41</f>
+        <v>49152</v>
       </c>
       <c r="J41" s="23" t="s">
-        <v>221</v>
+        <v>66</v>
       </c>
       <c r="L41" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M41" s="28">
         <v>32</v>
@@ -2971,328 +2972,184 @@
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B42" s="24"/>
-      <c r="C42" s="31"/>
+      <c r="C42" s="36" t="s">
+        <v>39</v>
+      </c>
       <c r="D42" s="23" t="str">
         <f>F41</f>
-        <v>0xAB00</v>
+        <v>0xC000</v>
       </c>
       <c r="E42" s="23" t="s">
-        <v>219</v>
+        <v>237</v>
       </c>
       <c r="F42" s="23" t="str">
-        <f t="shared" si="61"/>
-        <v>0xAC00</v>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I42))</f>
+        <v>0x10000</v>
       </c>
       <c r="G42" s="23">
         <f t="shared" si="62"/>
-        <v>43776</v>
+        <v>49152</v>
       </c>
       <c r="H42" s="23">
-        <f t="shared" si="63"/>
-        <v>256</v>
+        <f t="shared" si="62"/>
+        <v>16384</v>
       </c>
       <c r="I42" s="23">
-        <f t="shared" si="64"/>
-        <v>44032</v>
+        <f>G42+H42</f>
+        <v>65536</v>
       </c>
       <c r="J42" s="23" t="s">
-        <v>222</v>
+        <v>16</v>
       </c>
       <c r="L42" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M42" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B43" s="24"/>
-      <c r="C43" s="32"/>
-      <c r="D43" s="23" t="str">
-        <f>F42</f>
-        <v>0xAC00</v>
-      </c>
-      <c r="E43" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="F43" s="23" t="str">
-        <f t="shared" ref="F43" si="69">_xlfn.CONCAT("0x",DEC2HEX(I43))</f>
-        <v>0xAD00</v>
-      </c>
-      <c r="G43" s="23">
-        <f t="shared" ref="G43" si="70">HEX2DEC(MID(D43, 3, LEN(D43)-2))</f>
-        <v>44032</v>
-      </c>
-      <c r="H43" s="23">
-        <f t="shared" ref="H43" si="71">HEX2DEC(MID(E43, 3, LEN(E43)-2))</f>
-        <v>256</v>
-      </c>
-      <c r="I43" s="23">
-        <f t="shared" ref="I43" si="72">G43+H43</f>
-        <v>44288</v>
-      </c>
-      <c r="J43" s="23" t="s">
-        <v>223</v>
-      </c>
       <c r="L43" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M43" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B44" s="24"/>
-      <c r="C44" s="27"/>
-      <c r="D44" s="27" t="str">
-        <f>F43</f>
-        <v>0xAD00</v>
-      </c>
-      <c r="E44" s="27" t="s">
-        <v>220</v>
-      </c>
-      <c r="F44" s="27" t="str">
-        <f t="shared" si="61"/>
-        <v>0xB000</v>
-      </c>
-      <c r="G44" s="27">
-        <f t="shared" si="62"/>
-        <v>44288</v>
-      </c>
-      <c r="H44" s="27">
-        <f t="shared" si="63"/>
-        <v>768</v>
-      </c>
-      <c r="I44" s="27">
-        <f t="shared" si="64"/>
-        <v>45056</v>
-      </c>
-      <c r="J44" s="27" t="s">
-        <v>26</v>
+      <c r="B44" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="C44" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="D44" s="23" t="str">
+        <f>F42</f>
+        <v>0x10000</v>
+      </c>
+      <c r="E44" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M29))</f>
+        <v>0x100</v>
+      </c>
+      <c r="F44" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I44))</f>
+        <v>0x10100</v>
+      </c>
+      <c r="G44" s="23">
+        <f>HEX2DEC(MID(D44, 3, LEN(D44)-2))</f>
+        <v>65536</v>
+      </c>
+      <c r="H44" s="23">
+        <f>HEX2DEC(MID(E44, 3, LEN(E44)-2))</f>
+        <v>256</v>
+      </c>
+      <c r="I44" s="23">
+        <f>G44+H44</f>
+        <v>65792</v>
+      </c>
+      <c r="J44" s="23" t="s">
+        <v>44</v>
       </c>
       <c r="L44" s="18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M44" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B45" s="24"/>
-      <c r="C45" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="D45" s="23" t="str">
-        <f>F44</f>
-        <v>0xB000</v>
-      </c>
-      <c r="E45" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M52))</f>
-        <v>0x80</v>
-      </c>
-      <c r="F45" s="23" t="str">
-        <f t="shared" ref="F45:F46" si="73">_xlfn.CONCAT("0x",DEC2HEX(I45))</f>
-        <v>0xB080</v>
-      </c>
-      <c r="G45" s="23">
-        <f t="shared" ref="G45:G46" si="74">HEX2DEC(MID(D45, 3, LEN(D45)-2))</f>
-        <v>45056</v>
-      </c>
-      <c r="H45" s="23">
-        <f t="shared" ref="H45:H46" si="75">HEX2DEC(MID(E45, 3, LEN(E45)-2))</f>
-        <v>128</v>
-      </c>
-      <c r="I45" s="23">
-        <f t="shared" ref="I45:I46" si="76">G45+H45</f>
-        <v>45184</v>
-      </c>
-      <c r="J45" s="23" t="s">
-        <v>48</v>
+      <c r="B45" s="38" t="s">
+        <v>131</v>
       </c>
       <c r="L45" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M45" s="18">
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B46" s="24"/>
-      <c r="C46" s="34"/>
-      <c r="D46" s="27" t="str">
-        <f t="shared" si="2"/>
-        <v>0xB080</v>
-      </c>
-      <c r="E46" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="F46" s="27" t="str">
-        <f t="shared" si="73"/>
-        <v>0xB400</v>
-      </c>
-      <c r="G46" s="27">
-        <f t="shared" si="74"/>
-        <v>45184</v>
-      </c>
-      <c r="H46" s="27">
-        <f t="shared" si="75"/>
-        <v>896</v>
-      </c>
-      <c r="I46" s="27">
-        <f t="shared" si="76"/>
-        <v>46080</v>
-      </c>
-      <c r="J46" s="27" t="s">
-        <v>26</v>
-      </c>
+    <row r="46" spans="2:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="B46" s="38"/>
+      <c r="C46"/>
+      <c r="D46"/>
+      <c r="E46"/>
+      <c r="F46"/>
+      <c r="G46"/>
+      <c r="H46"/>
+      <c r="I46"/>
+      <c r="J46"/>
       <c r="L46" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="M46" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B47" s="24"/>
-      <c r="C47" s="34"/>
-      <c r="D47" s="23" t="str">
-        <f t="shared" ref="D47:D48" si="77">F46</f>
-        <v>0xB400</v>
-      </c>
+      <c r="B47" s="38"/>
+      <c r="C47" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="D47" s="23"/>
       <c r="E47" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M65))</f>
-        <v>0x4</v>
-      </c>
-      <c r="F47" s="23" t="str">
-        <f t="shared" ref="F47:F48" si="78">_xlfn.CONCAT("0x",DEC2HEX(I47))</f>
-        <v>0xB404</v>
-      </c>
-      <c r="G47" s="23">
-        <f t="shared" ref="G47:G48" si="79">HEX2DEC(MID(D47, 3, LEN(D47)-2))</f>
-        <v>46080</v>
-      </c>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M38))</f>
+        <v>0x4000</v>
+      </c>
+      <c r="F47" s="23"/>
+      <c r="G47" s="23"/>
       <c r="H47" s="23">
-        <f t="shared" ref="H47:H48" si="80">HEX2DEC(MID(E47, 3, LEN(E47)-2))</f>
-        <v>4</v>
-      </c>
-      <c r="I47" s="23">
-        <f t="shared" ref="I47:I48" si="81">G47+H47</f>
-        <v>46084</v>
-      </c>
+        <f>HEX2DEC(MID(E47, 3, LEN(E47)-2))</f>
+        <v>16384</v>
+      </c>
+      <c r="I47" s="23"/>
       <c r="J47" s="23" t="s">
-        <v>80</v>
+        <v>41</v>
       </c>
       <c r="L47" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M47" s="18">
         <v>9</v>
       </c>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B48" s="24"/>
-      <c r="C48" s="34"/>
-      <c r="D48" s="27" t="str">
-        <f t="shared" si="77"/>
-        <v>0xB404</v>
-      </c>
-      <c r="E48" s="27" t="s">
-        <v>121</v>
-      </c>
-      <c r="F48" s="27" t="str">
-        <f t="shared" si="78"/>
-        <v>0xB800</v>
-      </c>
-      <c r="G48" s="27">
-        <f t="shared" si="79"/>
-        <v>46084</v>
-      </c>
-      <c r="H48" s="27">
-        <f t="shared" si="80"/>
-        <v>1020</v>
-      </c>
-      <c r="I48" s="27">
-        <f t="shared" si="81"/>
-        <v>47104</v>
-      </c>
-      <c r="J48" s="27" t="s">
-        <v>26</v>
+      <c r="B48" s="38"/>
+      <c r="C48" s="35"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M71))</f>
+        <v>0x800</v>
+      </c>
+      <c r="F48" s="23"/>
+      <c r="G48" s="23"/>
+      <c r="H48" s="23">
+        <f>HEX2DEC(MID(E48, 3, LEN(E48)-2))</f>
+        <v>2048</v>
+      </c>
+      <c r="I48" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="J48" s="23" t="s">
+        <v>122</v>
       </c>
       <c r="L48" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M48" s="18">
         <v>7</v>
       </c>
     </row>
     <row r="49" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B49" s="24"/>
-      <c r="C49" s="35"/>
-      <c r="D49" s="23" t="str">
-        <f>F48</f>
-        <v>0xB800</v>
-      </c>
-      <c r="E49" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M59))</f>
-        <v>0x800</v>
-      </c>
-      <c r="F49" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I49))</f>
-        <v>0xC000</v>
-      </c>
-      <c r="G49" s="23">
-        <f t="shared" ref="G49:H50" si="82">HEX2DEC(MID(D49, 3, LEN(D49)-2))</f>
-        <v>47104</v>
-      </c>
-      <c r="H49" s="23">
-        <f t="shared" si="82"/>
-        <v>2048</v>
-      </c>
-      <c r="I49" s="23">
-        <f>G49+H49</f>
-        <v>49152</v>
-      </c>
-      <c r="J49" s="23" t="s">
-        <v>67</v>
-      </c>
+      <c r="B49" s="38"/>
       <c r="L49" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M49" s="18">
         <v>9</v>
       </c>
     </row>
     <row r="50" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B50" s="24"/>
-      <c r="C50" s="37" t="s">
-        <v>237</v>
-      </c>
-      <c r="D50" s="23" t="str">
-        <f>F49</f>
-        <v>0xC000</v>
-      </c>
-      <c r="E50" s="23" t="s">
-        <v>239</v>
-      </c>
-      <c r="F50" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I50))</f>
-        <v>0xE000</v>
-      </c>
-      <c r="G50" s="23">
-        <f t="shared" si="82"/>
-        <v>49152</v>
-      </c>
-      <c r="H50" s="23">
-        <f t="shared" si="82"/>
-        <v>8192</v>
-      </c>
-      <c r="I50" s="23">
-        <f>G50+H50</f>
-        <v>57344</v>
-      </c>
-      <c r="J50" s="23" t="s">
-        <v>238</v>
-      </c>
+      <c r="B50" s="38"/>
       <c r="L50" s="29" t="s">
         <v>4</v>
       </c>
@@ -3302,35 +3159,23 @@
       </c>
     </row>
     <row r="51" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B51" s="36"/>
-      <c r="C51" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="D51" s="23" t="str">
-        <f>F50</f>
-        <v>0xE000</v>
-      </c>
+      <c r="B51" s="38"/>
+      <c r="C51" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="D51" s="23"/>
       <c r="E51" s="23" t="s">
-        <v>239</v>
-      </c>
-      <c r="F51" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I51))</f>
-        <v>0x10000</v>
-      </c>
-      <c r="G51" s="23">
-        <f t="shared" ref="G51" si="83">HEX2DEC(MID(D51, 3, LEN(D51)-2))</f>
-        <v>57344</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="F51" s="23"/>
+      <c r="G51" s="23"/>
       <c r="H51" s="23">
-        <f t="shared" ref="H51" si="84">HEX2DEC(MID(E51, 3, LEN(E51)-2))</f>
-        <v>8192</v>
-      </c>
-      <c r="I51" s="23">
-        <f>G51+H51</f>
-        <v>65536</v>
-      </c>
+        <f t="shared" ref="H51" si="63">HEX2DEC(MID(E51, 3, LEN(E51)-2))</f>
+        <v>131072</v>
+      </c>
+      <c r="I51" s="23"/>
       <c r="J51" s="23" t="s">
-        <v>16</v>
+        <v>143</v>
       </c>
       <c r="L51" s="18" t="s">
         <v>3</v>
@@ -3341,8 +3186,26 @@
       </c>
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B52" s="38"/>
+      <c r="C52" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="D52" s="23"/>
+      <c r="E52" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="F52" s="23"/>
+      <c r="G52" s="23"/>
+      <c r="H52" s="23">
+        <f t="shared" ref="H52" si="64">HEX2DEC(MID(E52, 3, LEN(E52)-2))</f>
+        <v>65536</v>
+      </c>
+      <c r="I52" s="23"/>
+      <c r="J52" s="23" t="s">
+        <v>156</v>
+      </c>
       <c r="L52" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M52" s="29">
         <f>M41*M51</f>
@@ -3350,126 +3213,71 @@
       </c>
     </row>
     <row r="53" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B53" s="38" t="s">
-        <v>133</v>
-      </c>
-      <c r="C53" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="D53" s="23" t="str">
-        <f>F50</f>
-        <v>0xE000</v>
-      </c>
-      <c r="E53" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M29))</f>
-        <v>0x100</v>
-      </c>
-      <c r="F53" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I53))</f>
-        <v>0xE100</v>
-      </c>
-      <c r="G53" s="23">
-        <f>HEX2DEC(MID(D53, 3, LEN(D53)-2))</f>
-        <v>57344</v>
-      </c>
-      <c r="H53" s="23">
-        <f>HEX2DEC(MID(E53, 3, LEN(E53)-2))</f>
-        <v>256</v>
-      </c>
-      <c r="I53" s="23">
-        <f>G53+H53</f>
-        <v>57600</v>
-      </c>
-      <c r="J53" s="23" t="s">
-        <v>45</v>
-      </c>
+      <c r="B53" s="38"/>
     </row>
     <row r="54" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B54" s="39" t="s">
-        <v>132</v>
+      <c r="B54" s="38"/>
+      <c r="C54" s="36" t="s">
+        <v>230</v>
+      </c>
+      <c r="D54" s="23"/>
+      <c r="E54" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="F54" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I54))</f>
+        <v>0x10000</v>
+      </c>
+      <c r="G54" s="23"/>
+      <c r="H54" s="23">
+        <f t="shared" ref="H54" si="65">HEX2DEC(MID(E54, 3, LEN(E54)-2))</f>
+        <v>65536</v>
+      </c>
+      <c r="I54" s="23">
+        <f>G54+H54</f>
+        <v>65536</v>
+      </c>
+      <c r="J54" s="23" t="s">
+        <v>231</v>
       </c>
       <c r="L54" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M54" s="18" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="55" spans="2:16" ht="15" x14ac:dyDescent="0.25">
-      <c r="B55" s="39"/>
-      <c r="C55"/>
-      <c r="D55"/>
-      <c r="E55"/>
-      <c r="F55"/>
-      <c r="G55"/>
-      <c r="H55"/>
-      <c r="I55"/>
-      <c r="J55"/>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="55" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B55" s="38"/>
       <c r="L55" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M55" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="56" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B56" s="39"/>
-      <c r="C56" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="D56" s="23"/>
-      <c r="E56" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M38))</f>
-        <v>0x4000</v>
-      </c>
-      <c r="F56" s="23"/>
-      <c r="G56" s="23"/>
-      <c r="H56" s="23">
-        <f>HEX2DEC(MID(E56, 3, LEN(E56)-2))</f>
-        <v>16384</v>
-      </c>
-      <c r="I56" s="23"/>
-      <c r="J56" s="23" t="s">
-        <v>42</v>
-      </c>
+      <c r="B56" s="38"/>
       <c r="L56" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M56" s="18">
         <v>512</v>
       </c>
     </row>
     <row r="57" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B57" s="39"/>
-      <c r="C57" s="35"/>
-      <c r="D57" s="23"/>
-      <c r="E57" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M71))</f>
-        <v>0x800</v>
-      </c>
-      <c r="F57" s="23"/>
-      <c r="G57" s="23"/>
-      <c r="H57" s="23">
-        <f>HEX2DEC(MID(E57, 3, LEN(E57)-2))</f>
-        <v>2048</v>
-      </c>
-      <c r="I57" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="J57" s="23" t="s">
-        <v>123</v>
-      </c>
+      <c r="B57" s="38"/>
       <c r="L57" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M57" s="28">
         <v>16</v>
       </c>
     </row>
     <row r="58" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B58" s="39"/>
+      <c r="B58" s="38"/>
       <c r="L58" s="18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M58" s="18">
         <f>M55*M56*M57</f>
@@ -3477,9 +3285,9 @@
       </c>
     </row>
     <row r="59" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B59" s="39"/>
+      <c r="B59" s="38"/>
       <c r="L59" s="18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M59" s="18">
         <f>M58/8</f>
@@ -3487,58 +3295,24 @@
       </c>
     </row>
     <row r="60" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B60" s="39"/>
-      <c r="C60" s="40" t="s">
-        <v>144</v>
-      </c>
-      <c r="D60" s="23"/>
-      <c r="E60" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="F60" s="23"/>
-      <c r="G60" s="23"/>
-      <c r="H60" s="23">
-        <f t="shared" ref="H60" si="85">HEX2DEC(MID(E60, 3, LEN(E60)-2))</f>
-        <v>131072</v>
-      </c>
-      <c r="I60" s="23"/>
-      <c r="J60" s="23" t="s">
-        <v>144</v>
-      </c>
+      <c r="B60" s="38"/>
     </row>
     <row r="61" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B61" s="39"/>
-      <c r="C61" s="40" t="s">
-        <v>157</v>
-      </c>
-      <c r="D61" s="23"/>
-      <c r="E61" s="23" t="s">
-        <v>158</v>
-      </c>
-      <c r="F61" s="23"/>
-      <c r="G61" s="23"/>
-      <c r="H61" s="23">
-        <f t="shared" ref="H61" si="86">HEX2DEC(MID(E61, 3, LEN(E61)-2))</f>
-        <v>65536</v>
-      </c>
-      <c r="I61" s="23"/>
-      <c r="J61" s="23" t="s">
-        <v>157</v>
-      </c>
+      <c r="B61" s="38"/>
       <c r="L61" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M61" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P61" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="62" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B62" s="39"/>
+      <c r="B62" s="38"/>
       <c r="L62" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M62" s="18">
         <v>32</v>
@@ -3549,30 +3323,7 @@
       </c>
     </row>
     <row r="63" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B63" s="39"/>
-      <c r="C63" s="37" t="s">
-        <v>237</v>
-      </c>
-      <c r="D63" s="23"/>
-      <c r="E63" s="23" t="s">
-        <v>158</v>
-      </c>
-      <c r="F63" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I63))</f>
-        <v>0x10000</v>
-      </c>
-      <c r="G63" s="23"/>
-      <c r="H63" s="23">
-        <f t="shared" ref="H63" si="87">HEX2DEC(MID(E63, 3, LEN(E63)-2))</f>
-        <v>65536</v>
-      </c>
-      <c r="I63" s="23">
-        <f>G63+H63</f>
-        <v>65536</v>
-      </c>
-      <c r="J63" s="23" t="s">
-        <v>238</v>
-      </c>
+      <c r="B63" s="38"/>
       <c r="L63" s="28" t="s">
         <v>4</v>
       </c>
@@ -3581,9 +3332,9 @@
       </c>
     </row>
     <row r="64" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B64" s="39"/>
+      <c r="B64" s="38"/>
       <c r="L64" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M64" s="18">
         <f>M62*M63</f>
@@ -3591,9 +3342,9 @@
       </c>
     </row>
     <row r="65" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B65" s="39"/>
+      <c r="B65" s="38"/>
       <c r="L65" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M65" s="18">
         <f>M64/8</f>
@@ -3601,45 +3352,42 @@
       </c>
     </row>
     <row r="66" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B66" s="39"/>
+      <c r="B66" s="38"/>
     </row>
     <row r="67" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B67" s="39"/>
+      <c r="B67" s="40"/>
       <c r="L67" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="M67" s="18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="68" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L68" s="18" t="s">
         <v>123</v>
-      </c>
-      <c r="M67" s="18" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="68" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B68" s="39"/>
-      <c r="L68" s="18" t="s">
-        <v>124</v>
       </c>
       <c r="M68" s="18">
         <v>512</v>
       </c>
       <c r="N68" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="69" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B69" s="39"/>
       <c r="L69" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M69" s="28">
         <v>32</v>
       </c>
       <c r="N69" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="70" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B70" s="39"/>
       <c r="L70" s="29" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M70" s="18">
         <f>M68*M69</f>
@@ -3647,46 +3395,38 @@
       </c>
     </row>
     <row r="71" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B71" s="39"/>
       <c r="L71" s="18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M71" s="18">
         <f>M70/8</f>
         <v>2048</v>
       </c>
     </row>
-    <row r="72" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B72" s="39"/>
-    </row>
     <row r="73" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B73" s="39"/>
       <c r="L73" s="20" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="74" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B74" s="39"/>
       <c r="L74" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M74" s="18">
         <v>8</v>
       </c>
     </row>
     <row r="75" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B75" s="39"/>
       <c r="L75" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M75" s="18">
         <v>8</v>
       </c>
     </row>
     <row r="76" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B76" s="41"/>
       <c r="L76" s="18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M76" s="18">
         <v>8</v>
@@ -3694,23 +3434,23 @@
     </row>
     <row r="77" spans="2:14" x14ac:dyDescent="0.2">
       <c r="L77" s="18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M77" s="18">
         <v>8</v>
       </c>
     </row>
     <row r="78" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="L78" s="43" t="s">
-        <v>153</v>
-      </c>
-      <c r="M78" s="43">
+      <c r="L78" s="42" t="s">
+        <v>152</v>
+      </c>
+      <c r="M78" s="42">
         <v>96</v>
       </c>
     </row>
     <row r="79" spans="2:14" x14ac:dyDescent="0.2">
       <c r="L79" s="29" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M79" s="29">
         <f>SUM(M74:M78)</f>
@@ -3719,7 +3459,7 @@
     </row>
     <row r="80" spans="2:14" x14ac:dyDescent="0.2">
       <c r="L80" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M80" s="18">
         <f>M79/8</f>
@@ -3728,34 +3468,34 @@
     </row>
     <row r="82" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L82" s="20" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="83" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L83" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="M83" s="18">
         <v>32</v>
       </c>
       <c r="N83" s="18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="84" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L84" s="18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M84" s="18">
         <v>24</v>
       </c>
       <c r="N84" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="85" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L85" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M85" s="18">
         <v>8</v>
@@ -3763,7 +3503,7 @@
     </row>
     <row r="86" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L86" s="29" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="M86" s="29">
         <f>M83*M84*M85</f>
@@ -3772,7 +3512,7 @@
     </row>
     <row r="87" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L87" s="18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M87" s="18">
         <f>M86/8</f>
@@ -3781,12 +3521,12 @@
     </row>
     <row r="89" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L89" s="20" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="90" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L90" s="28" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M90" s="28">
         <v>64</v>
@@ -3794,7 +3534,7 @@
     </row>
     <row r="91" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L91" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M91" s="18">
         <v>16</v>
@@ -3802,7 +3542,7 @@
     </row>
     <row r="92" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L92" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M92" s="18">
         <v>16</v>
@@ -3810,18 +3550,18 @@
     </row>
     <row r="93" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L93" s="18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="M93" s="18">
         <v>16</v>
       </c>
       <c r="N93" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="94" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L94" s="29" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="M94" s="29">
         <f>M91*M92*M93</f>
@@ -3830,7 +3570,7 @@
     </row>
     <row r="95" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L95" s="18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="M95" s="18">
         <f>M94/8</f>
@@ -3839,7 +3579,7 @@
     </row>
     <row r="96" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L96" s="29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="M96" s="29">
         <f>M90*M95</f>
@@ -3848,8 +3588,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C21:C22"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3877,10 +3617,10 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.35">
@@ -3889,189 +3629,189 @@
     </row>
     <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" s="15" t="s">
         <v>115</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>69</v>
-      </c>
       <c r="G4" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>85</v>
-      </c>
       <c r="F6" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>98</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>109</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>111</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I22" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I23" s="41" t="s">
         <v>149</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I23" s="42" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -4096,13 +3836,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" t="s">
         <v>161</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>162</v>
-      </c>
-      <c r="C1" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4147,10 +3887,10 @@
         <v>272</v>
       </c>
       <c r="D1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" t="s">
         <v>164</v>
-      </c>
-      <c r="E1" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -4173,18 +3913,18 @@
         <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -4213,23 +3953,23 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
-        <v>225</v>
+      <c r="A2" s="41" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="B4" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="C4" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -4237,10 +3977,10 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="C5" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -4248,10 +3988,10 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="C6" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -4259,7 +3999,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4267,7 +4007,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -4275,7 +4015,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -4283,7 +4023,7 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>